<commit_message>
update Survey after 2nd iteration (14 05 2021)
</commit_message>
<xml_diff>
--- a/Survey.xlsx
+++ b/Survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo.sharepoint.com/sites/polifonia/Shared Documents/WP1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3F6DFF8-2FEE-43F4-BB82-CC550090378F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0559A1C3-9399-4CEE-AC20-2FFB00A965EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="460" windowWidth="32020" windowHeight="25420" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="460" windowWidth="32020" windowHeight="25420" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -11675,8 +11675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B81DAE-D652-4BB6-8C73-F96210539325}">
   <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="M3" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -11790,7 +11790,7 @@
         <v>165</v>
       </c>
       <c r="B3" s="102" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="114" t="s">
@@ -13616,7 +13616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF55BB61-3A6F-4270-90C9-AB8A8506205C}">
   <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -14846,6 +14846,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A444E4101166CB49B259A75BDE06F3BF" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1da9179d651506a4ee704055c7c7620">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b3e41e30-95eb-45b9-b657-d2eda7f0eaf6" xmlns:ns3="d6ffb985-a7ae-40c0-906d-05d0dcf51054" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="22336762794d641df60944ca434000c5" ns2:_="" ns3:_="">
     <xsd:import namespace="b3e41e30-95eb-45b9-b657-d2eda7f0eaf6"/>
@@ -15056,23 +15065,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B45268-2425-47D2-956B-0CCF1D385955}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D05AB7-5B37-4680-A3C6-E19CC68A6CA4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1918471B-3575-494A-A238-97D47571C991}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1918471B-3575-494A-A238-97D47571C991}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D05AB7-5B37-4680-A3C6-E19CC68A6CA4}"/>
 </file>
</xml_diff>

<commit_message>
reorganized formats and standards in technical part
</commit_message>
<xml_diff>
--- a/Survey.xlsx
+++ b/Survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveunibo.sharepoint.com/sites/polifonia/Shared Documents/WP1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe/Documents/GitHub/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0559A1C3-9399-4CEE-AC20-2FFB00A965EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D0A178-A7CA-1440-896B-20125A47A610}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="460" windowWidth="32020" windowHeight="25420" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1580" yWindow="460" windowWidth="32020" windowHeight="12460" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -25,26 +25,17 @@
     <sheet name="SOCIO-PEDAGOGICAL PART" sheetId="10" r:id="rId10"/>
     <sheet name="OTHER" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3013" uniqueCount="610">
   <si>
     <t>Colonne1</t>
   </si>
@@ -2039,12 +2030,43 @@
   <si>
     <t>Yes, definitely with TONALITIES</t>
   </si>
+  <si>
+    <t>XML, RDF, MAG and other formats</t>
+  </si>
+  <si>
+    <t>TXT, MIDI</t>
+  </si>
+  <si>
+    <t>MEI, MusicXML</t>
+  </si>
+  <si>
+    <t>CSC</t>
+  </si>
+  <si>
+    <t>RDF, Turtle</t>
+  </si>
+  <si>
+    <t>ArCo, Unimarc</t>
+  </si>
+  <si>
+    <t>JPEG, TIFF, XML, RDF, various sound formats</t>
+  </si>
+  <si>
+    <t>DOC, DOCX, WP5</t>
+  </si>
+  <si>
+    <t>TAR, GZIP, RDF, N-triples, RDF, RDFS, OWL</t>
+  </si>
+  <si>
+    <t>KERN, MIDI, PDF, PNG, JPG, TXT, Lilypond, MP3, HUMDRUM
+See: http://www.liederenbank.nl/mtc/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2057,7 +2079,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2071,7 +2093,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2101,7 +2123,7 @@
       <sz val="11"/>
       <color rgb="FF548235"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2156,6 +2178,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2167,12 +2190,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2225,7 +2249,7 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="26">
@@ -4077,12 +4101,12 @@
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="35" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="35" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="35" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="8" customFormat="1" ht="80.099999999999994" hidden="1">
+    <row r="1" spans="1:61" s="8" customFormat="1" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
@@ -4256,7 +4280,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:61" s="29" customFormat="1" ht="29.25" customHeight="1">
+    <row r="2" spans="1:61" s="29" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
         <v>57</v>
       </c>
@@ -4436,7 +4460,7 @@
       </c>
       <c r="BH2" s="28"/>
     </row>
-    <row r="3" spans="1:61" s="27" customFormat="1" ht="93" customHeight="1">
+    <row r="3" spans="1:61" s="27" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>63</v>
       </c>
@@ -4615,7 +4639,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:61" s="27" customFormat="1" ht="80.099999999999994">
+    <row r="4" spans="1:61" s="27" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>90</v>
       </c>
@@ -4760,7 +4784,7 @@
       <c r="BF4" s="24"/>
       <c r="BG4" s="31"/>
     </row>
-    <row r="5" spans="1:61" s="27" customFormat="1" ht="159.94999999999999">
+    <row r="5" spans="1:61" s="27" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>109</v>
       </c>
@@ -4885,7 +4909,7 @@
       <c r="BF5" s="24"/>
       <c r="BG5" s="31"/>
     </row>
-    <row r="6" spans="1:61" s="27" customFormat="1" ht="128.1">
+    <row r="6" spans="1:61" s="27" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>125</v>
       </c>
@@ -4998,7 +5022,7 @@
       <c r="BF6" s="24"/>
       <c r="BG6" s="31"/>
     </row>
-    <row r="7" spans="1:61" ht="320.10000000000002">
+    <row r="7" spans="1:61" ht="320" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>136</v>
       </c>
@@ -5122,7 +5146,7 @@
       <c r="BF7" s="9"/>
       <c r="BG7" s="9"/>
     </row>
-    <row r="8" spans="1:61" ht="15.95">
+    <row r="8" spans="1:61" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
         <v>165</v>
       </c>
@@ -5191,7 +5215,7 @@
       <c r="BF8" s="9"/>
       <c r="BG8" s="9"/>
     </row>
-    <row r="9" spans="1:61" ht="80.099999999999994">
+    <row r="9" spans="1:61" ht="80" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>165</v>
       </c>
@@ -5310,7 +5334,7 @@
       <c r="BF9" s="9"/>
       <c r="BG9" s="9"/>
     </row>
-    <row r="10" spans="1:61" ht="15.95">
+    <row r="10" spans="1:61" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>165</v>
       </c>
@@ -5394,7 +5418,7 @@
       <c r="BF10" s="9"/>
       <c r="BG10" s="9"/>
     </row>
-    <row r="11" spans="1:61" ht="176.1">
+    <row r="11" spans="1:61" ht="176" x14ac:dyDescent="0.2">
       <c r="B11" s="43" t="s">
         <v>198</v>
       </c>
@@ -5557,7 +5581,7 @@
       <c r="BG11" s="44"/>
       <c r="BH11" s="46"/>
     </row>
-    <row r="12" spans="1:61" ht="96">
+    <row r="12" spans="1:61" ht="96" x14ac:dyDescent="0.2">
       <c r="B12" s="36" t="s">
         <v>233</v>
       </c>
@@ -5716,7 +5740,7 @@
       <c r="BG12" s="47"/>
       <c r="BH12" s="45"/>
     </row>
-    <row r="13" spans="1:61" ht="176.1">
+    <row r="13" spans="1:61" ht="176" x14ac:dyDescent="0.2">
       <c r="B13" s="43" t="s">
         <v>256</v>
       </c>
@@ -5888,7 +5912,7 @@
       <c r="BH13" s="45"/>
       <c r="BI13" s="45"/>
     </row>
-    <row r="14" spans="1:61" ht="409.6">
+    <row r="14" spans="1:61" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B14" s="36" t="s">
         <v>289</v>
       </c>
@@ -6045,7 +6069,7 @@
       <c r="BG14" s="47"/>
       <c r="BH14" s="46"/>
     </row>
-    <row r="15" spans="1:61" ht="176.1">
+    <row r="15" spans="1:61" ht="176" x14ac:dyDescent="0.2">
       <c r="B15" s="43" t="s">
         <v>328</v>
       </c>
@@ -6210,7 +6234,7 @@
       </c>
       <c r="BH15" s="46"/>
     </row>
-    <row r="16" spans="1:61" ht="128.1">
+    <row r="16" spans="1:61" ht="128" x14ac:dyDescent="0.2">
       <c r="B16" s="36" t="s">
         <v>370</v>
       </c>
@@ -6373,7 +6397,7 @@
       <c r="BG16" s="47"/>
       <c r="BH16" s="46"/>
     </row>
-    <row r="17" spans="2:62" ht="176.1">
+    <row r="17" spans="2:62" ht="176" x14ac:dyDescent="0.2">
       <c r="B17" s="43" t="s">
         <v>413</v>
       </c>
@@ -6536,7 +6560,7 @@
       <c r="BG17" s="44"/>
       <c r="BH17" s="46"/>
     </row>
-    <row r="18" spans="2:62" ht="111.95">
+    <row r="18" spans="2:62" ht="112" x14ac:dyDescent="0.2">
       <c r="B18" s="36" t="s">
         <v>456</v>
       </c>
@@ -6711,25 +6735,25 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="62.25" customHeight="1">
+    <row r="1" spans="1:14" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="144"/>
       <c r="B1" s="145" t="s">
         <v>84</v>
@@ -6743,7 +6767,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="48" customHeight="1">
+    <row r="2" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="113" t="s">
         <v>136</v>
       </c>
@@ -6763,7 +6787,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="33" customHeight="1">
+    <row r="3" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="114" t="s">
         <v>165</v>
       </c>
@@ -6781,7 +6805,7 @@
       </c>
       <c r="H3" s="102"/>
     </row>
-    <row r="4" spans="1:14" ht="32.25" customHeight="1">
+    <row r="4" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="115" t="s">
         <v>198</v>
       </c>
@@ -6799,7 +6823,7 @@
       </c>
       <c r="H4" s="103"/>
     </row>
-    <row r="5" spans="1:14" ht="33" customHeight="1">
+    <row r="5" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="116" t="s">
         <v>233</v>
       </c>
@@ -6817,7 +6841,7 @@
       </c>
       <c r="H5" s="104"/>
     </row>
-    <row r="6" spans="1:14" ht="78.75" customHeight="1">
+    <row r="6" spans="1:14" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115" t="s">
         <v>256</v>
       </c>
@@ -6837,7 +6861,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="48.75" customHeight="1">
+    <row r="7" spans="1:14" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="116" t="s">
         <v>289</v>
       </c>
@@ -6857,7 +6881,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="49.5" customHeight="1">
+    <row r="8" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115" t="s">
         <v>328</v>
       </c>
@@ -6875,7 +6899,7 @@
       </c>
       <c r="H8" s="103"/>
     </row>
-    <row r="9" spans="1:14" ht="77.25" customHeight="1">
+    <row r="9" spans="1:14" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="116" t="s">
         <v>370</v>
       </c>
@@ -6893,7 +6917,7 @@
       </c>
       <c r="H9" s="104"/>
     </row>
-    <row r="10" spans="1:14" ht="51" customHeight="1">
+    <row r="10" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="115" t="s">
         <v>413</v>
       </c>
@@ -6913,7 +6937,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="36.75" customHeight="1">
+    <row r="11" spans="1:14" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="117" t="s">
         <v>456</v>
       </c>
@@ -6931,7 +6955,7 @@
       </c>
       <c r="H11" s="105"/>
     </row>
-    <row r="13" spans="1:14" ht="159.94999999999999">
+    <row r="13" spans="1:14" ht="160" x14ac:dyDescent="0.2">
       <c r="A13" s="146"/>
       <c r="B13" s="147" t="s">
         <v>85</v>
@@ -6953,7 +6977,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="48">
+    <row r="14" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="113" t="s">
         <v>136</v>
       </c>
@@ -6977,7 +7001,7 @@
       </c>
       <c r="N14" s="111"/>
     </row>
-    <row r="15" spans="1:14" ht="63.95">
+    <row r="15" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="114" t="s">
         <v>165</v>
       </c>
@@ -7005,7 +7029,7 @@
       </c>
       <c r="N15" s="102"/>
     </row>
-    <row r="16" spans="1:14" ht="48">
+    <row r="16" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="115" t="s">
         <v>198</v>
       </c>
@@ -7033,7 +7057,7 @@
       </c>
       <c r="N16" s="103"/>
     </row>
-    <row r="17" spans="1:14" ht="15.95">
+    <row r="17" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="116" t="s">
         <v>233</v>
       </c>
@@ -7061,7 +7085,7 @@
       </c>
       <c r="N17" s="104"/>
     </row>
-    <row r="18" spans="1:14" ht="111.95">
+    <row r="18" spans="1:14" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="115" t="s">
         <v>256</v>
       </c>
@@ -7091,7 +7115,7 @@
       </c>
       <c r="N18" s="103"/>
     </row>
-    <row r="19" spans="1:14" ht="60">
+    <row r="19" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="116" t="s">
         <v>289</v>
       </c>
@@ -7117,7 +7141,7 @@
       </c>
       <c r="N19" s="104"/>
     </row>
-    <row r="20" spans="1:14" ht="128.1">
+    <row r="20" spans="1:14" ht="128" x14ac:dyDescent="0.2">
       <c r="A20" s="115" t="s">
         <v>328</v>
       </c>
@@ -7145,7 +7169,7 @@
       </c>
       <c r="N20" s="103"/>
     </row>
-    <row r="21" spans="1:14" ht="144">
+    <row r="21" spans="1:14" ht="144" x14ac:dyDescent="0.2">
       <c r="A21" s="116" t="s">
         <v>370</v>
       </c>
@@ -7175,7 +7199,7 @@
       </c>
       <c r="N21" s="104"/>
     </row>
-    <row r="22" spans="1:14" ht="60">
+    <row r="22" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="115" t="s">
         <v>413</v>
       </c>
@@ -7203,7 +7227,7 @@
       </c>
       <c r="N22" s="103"/>
     </row>
-    <row r="23" spans="1:14" ht="48">
+    <row r="23" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="117" t="s">
         <v>456</v>
       </c>
@@ -7242,43 +7266,43 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.95">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="148"/>
       <c r="B1" s="149" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.95">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="113" t="s">
         <v>136</v>
       </c>
       <c r="B2" s="111"/>
     </row>
-    <row r="3" spans="1:2" ht="15.95">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="114" t="s">
         <v>165</v>
       </c>
       <c r="B3" s="102"/>
     </row>
-    <row r="4" spans="1:2" ht="15.95">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="115" t="s">
         <v>198</v>
       </c>
       <c r="B4" s="103"/>
     </row>
-    <row r="5" spans="1:2" ht="15.95">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="116" t="s">
         <v>233</v>
       </c>
       <c r="B5" s="104"/>
     </row>
-    <row r="6" spans="1:2" ht="15.95">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="115" t="s">
         <v>256</v>
       </c>
@@ -7286,13 +7310,13 @@
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.95">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="116" t="s">
         <v>289</v>
       </c>
       <c r="B7" s="104"/>
     </row>
-    <row r="8" spans="1:2" ht="111.75" customHeight="1">
+    <row r="8" spans="1:2" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115" t="s">
         <v>328</v>
       </c>
@@ -7300,19 +7324,19 @@
         <v>369</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.95">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="116" t="s">
         <v>370</v>
       </c>
       <c r="B9" s="104"/>
     </row>
-    <row r="10" spans="1:2" ht="15.95">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="115" t="s">
         <v>413</v>
       </c>
       <c r="B10" s="103"/>
     </row>
-    <row r="11" spans="1:2" ht="15.95">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="117" t="s">
         <v>456</v>
       </c>
@@ -7332,12 +7356,12 @@
       <selection pane="bottomLeft" activeCell="BG1" sqref="BG1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="35" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="35" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="35" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" s="27" customFormat="1" ht="176.1">
+    <row r="1" spans="1:62" s="27" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>497</v>
       </c>
@@ -7516,7 +7540,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="320.10000000000002">
+    <row r="2" spans="1:62" ht="320" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
         <v>136</v>
       </c>
@@ -7640,7 +7664,7 @@
       <c r="BF2" s="9"/>
       <c r="BG2" s="9"/>
     </row>
-    <row r="3" spans="1:62" s="51" customFormat="1" ht="303.95">
+    <row r="3" spans="1:62" s="51" customFormat="1" ht="304" x14ac:dyDescent="0.2">
       <c r="B3" s="51" t="s">
         <v>165</v>
       </c>
@@ -7774,7 +7798,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:62" ht="176.1">
+    <row r="4" spans="1:62" ht="176" x14ac:dyDescent="0.2">
       <c r="A4" s="51"/>
       <c r="B4" s="43" t="s">
         <v>198</v>
@@ -7940,7 +7964,7 @@
       <c r="BI4" s="51"/>
       <c r="BJ4" s="51"/>
     </row>
-    <row r="5" spans="1:62" ht="96">
+    <row r="5" spans="1:62" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="51"/>
       <c r="B5" s="54" t="s">
         <v>233</v>
@@ -8102,7 +8126,7 @@
       <c r="BI5" s="51"/>
       <c r="BJ5" s="51"/>
     </row>
-    <row r="6" spans="1:62" ht="176.1">
+    <row r="6" spans="1:62" ht="176" x14ac:dyDescent="0.2">
       <c r="A6" s="51"/>
       <c r="B6" s="43" t="s">
         <v>256</v>
@@ -8276,7 +8300,7 @@
       <c r="BI6" s="57"/>
       <c r="BJ6" s="51"/>
     </row>
-    <row r="7" spans="1:62" ht="409.6">
+    <row r="7" spans="1:62" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" s="51"/>
       <c r="B7" s="54" t="s">
         <v>289</v>
@@ -8436,7 +8460,7 @@
       <c r="BI7" s="51"/>
       <c r="BJ7" s="51"/>
     </row>
-    <row r="8" spans="1:62" ht="176.1">
+    <row r="8" spans="1:62" ht="176" x14ac:dyDescent="0.2">
       <c r="A8" s="51"/>
       <c r="B8" s="43" t="s">
         <v>328</v>
@@ -8604,7 +8628,7 @@
       <c r="BI8" s="51"/>
       <c r="BJ8" s="51"/>
     </row>
-    <row r="9" spans="1:62" ht="128.1">
+    <row r="9" spans="1:62" ht="128" x14ac:dyDescent="0.2">
       <c r="A9" s="51"/>
       <c r="B9" s="54" t="s">
         <v>370</v>
@@ -8770,7 +8794,7 @@
       <c r="BI9" s="51"/>
       <c r="BJ9" s="51"/>
     </row>
-    <row r="10" spans="1:62" ht="176.1">
+    <row r="10" spans="1:62" ht="176" x14ac:dyDescent="0.2">
       <c r="A10" s="51"/>
       <c r="B10" s="43" t="s">
         <v>413</v>
@@ -8936,7 +8960,7 @@
       <c r="BI10" s="51"/>
       <c r="BJ10" s="51"/>
     </row>
-    <row r="11" spans="1:62" ht="111.95">
+    <row r="11" spans="1:62" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="51"/>
       <c r="B11" s="54" t="s">
         <v>456</v>
@@ -9092,7 +9116,7 @@
       <c r="BI11" s="46"/>
       <c r="BJ11" s="46"/>
     </row>
-    <row r="37" spans="1:60" s="8" customFormat="1" ht="80.099999999999994" hidden="1">
+    <row r="37" spans="1:60" s="8" customFormat="1" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>0</v>
       </c>
@@ -9266,7 +9290,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:60" s="29" customFormat="1" ht="29.25" hidden="1" customHeight="1">
+    <row r="38" spans="1:60" s="29" customFormat="1" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="23" t="s">
         <v>57</v>
       </c>
@@ -9446,7 +9470,7 @@
       </c>
       <c r="BH38" s="28"/>
     </row>
-    <row r="39" spans="1:60" s="27" customFormat="1" ht="93" hidden="1" customHeight="1">
+    <row r="39" spans="1:60" s="27" customFormat="1" ht="93" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="23" t="s">
         <v>63</v>
       </c>
@@ -9625,7 +9649,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:60" s="27" customFormat="1" ht="80.099999999999994" hidden="1">
+    <row r="40" spans="1:60" s="27" customFormat="1" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="23" t="s">
         <v>90</v>
       </c>
@@ -9762,7 +9786,7 @@
       <c r="BF40" s="24"/>
       <c r="BG40" s="31"/>
     </row>
-    <row r="41" spans="1:60" s="27" customFormat="1" ht="159.94999999999999" hidden="1">
+    <row r="41" spans="1:60" s="27" customFormat="1" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="23" t="s">
         <v>109</v>
       </c>
@@ -9875,7 +9899,7 @@
       <c r="BF41" s="24"/>
       <c r="BG41" s="31"/>
     </row>
-    <row r="42" spans="1:60" s="27" customFormat="1" hidden="1">
+    <row r="42" spans="1:60" s="27" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="23"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -9955,20 +9979,20 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" customWidth="1"/>
-    <col min="3" max="3" width="80.42578125" customWidth="1"/>
-    <col min="4" max="4" width="50.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="51.5" customWidth="1"/>
+    <col min="3" max="3" width="80.5" customWidth="1"/>
+    <col min="4" max="4" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="71" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.100000000000001">
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="72"/>
       <c r="B2" s="70" t="s">
         <v>110</v>
@@ -9977,7 +10001,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.100000000000001">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="66" t="s">
         <v>136</v>
       </c>
@@ -9988,7 +10012,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="33.950000000000003">
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="66" t="s">
         <v>165</v>
       </c>
@@ -9999,7 +10023,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.100000000000001">
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="66" t="s">
         <v>198</v>
       </c>
@@ -10010,7 +10034,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.100000000000001">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="66" t="s">
         <v>233</v>
       </c>
@@ -10019,7 +10043,7 @@
       </c>
       <c r="C6" s="66"/>
     </row>
-    <row r="7" spans="1:3" ht="17.100000000000001">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="66" t="s">
         <v>256</v>
       </c>
@@ -10030,7 +10054,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="66" t="s">
         <v>289</v>
       </c>
@@ -10041,7 +10065,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.100000000000001">
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="66" t="s">
         <v>328</v>
       </c>
@@ -10052,7 +10076,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.100000000000001">
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="66" t="s">
         <v>370</v>
       </c>
@@ -10063,7 +10087,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.100000000000001">
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="66" t="s">
         <v>413</v>
       </c>
@@ -10074,7 +10098,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17.100000000000001">
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="66" t="s">
         <v>456</v>
       </c>
@@ -10085,13 +10109,13 @@
         <v>458</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.100000000000001">
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="72"/>
       <c r="B15" s="70" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="63.95">
+    <row r="16" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="66" t="s">
         <v>136</v>
       </c>
@@ -10099,7 +10123,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="84.95">
+    <row r="17" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="66" t="s">
         <v>165</v>
       </c>
@@ -10107,7 +10131,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="33.950000000000003">
+    <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="66" t="s">
         <v>198</v>
       </c>
@@ -10115,7 +10139,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.100000000000001">
+    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="66" t="s">
         <v>233</v>
       </c>
@@ -10123,7 +10147,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.100000000000001">
+    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="66" t="s">
         <v>256</v>
       </c>
@@ -10131,7 +10155,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17.100000000000001">
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="66" t="s">
         <v>289</v>
       </c>
@@ -10139,7 +10163,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="33.950000000000003">
+    <row r="22" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="66" t="s">
         <v>328</v>
       </c>
@@ -10147,7 +10171,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="68.099999999999994">
+    <row r="23" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="66" t="s">
         <v>370</v>
       </c>
@@ -10155,7 +10179,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1">
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="66" t="s">
         <v>413</v>
       </c>
@@ -10163,7 +10187,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="51">
+    <row r="25" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="66" t="s">
         <v>456</v>
       </c>
@@ -10171,13 +10195,13 @@
         <v>526</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17.100000000000001">
+    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="72"/>
       <c r="B28" s="70" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="96">
+    <row r="29" spans="1:2" ht="96" x14ac:dyDescent="0.2">
       <c r="A29" s="66" t="s">
         <v>136</v>
       </c>
@@ -10185,7 +10209,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="17.100000000000001">
+    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="66" t="s">
         <v>165</v>
       </c>
@@ -10193,7 +10217,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="51">
+    <row r="31" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="66" t="s">
         <v>198</v>
       </c>
@@ -10201,7 +10225,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="51">
+    <row r="32" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="66" t="s">
         <v>233</v>
       </c>
@@ -10209,7 +10233,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="51">
+    <row r="33" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="66" t="s">
         <v>256</v>
       </c>
@@ -10217,7 +10241,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="119.1">
+    <row r="34" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A34" s="66" t="s">
         <v>289</v>
       </c>
@@ -10225,7 +10249,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="51">
+    <row r="35" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="66" t="s">
         <v>328</v>
       </c>
@@ -10233,7 +10257,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="51">
+    <row r="36" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="66" t="s">
         <v>370</v>
       </c>
@@ -10241,7 +10265,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="51">
+    <row r="37" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="66" t="s">
         <v>413</v>
       </c>
@@ -10249,7 +10273,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="68.099999999999994">
+    <row r="38" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A38" s="66" t="s">
         <v>456</v>
       </c>
@@ -10257,13 +10281,13 @@
         <v>462</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17.100000000000001">
+    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="72"/>
       <c r="B40" s="70" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="80.099999999999994">
+    <row r="41" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A41" s="66" t="s">
         <v>136</v>
       </c>
@@ -10271,7 +10295,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="33.950000000000003">
+    <row r="42" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="66" t="s">
         <v>165</v>
       </c>
@@ -10279,7 +10303,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="17.100000000000001">
+    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="66" t="s">
         <v>198</v>
       </c>
@@ -10287,7 +10311,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17.100000000000001">
+    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="66" t="s">
         <v>233</v>
       </c>
@@ -10295,7 +10319,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17.100000000000001">
+    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="66" t="s">
         <v>256</v>
       </c>
@@ -10303,7 +10327,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="51">
+    <row r="46" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="66" t="s">
         <v>289</v>
       </c>
@@ -10311,7 +10335,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="51">
+    <row r="47" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="66" t="s">
         <v>328</v>
       </c>
@@ -10319,7 +10343,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17.100000000000001">
+    <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="66" t="s">
         <v>370</v>
       </c>
@@ -10327,7 +10351,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="33.950000000000003">
+    <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="66" t="s">
         <v>413</v>
       </c>
@@ -10335,19 +10359,19 @@
         <v>419</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="17.100000000000001">
+    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="66" t="s">
         <v>456</v>
       </c>
       <c r="B50" s="66"/>
     </row>
-    <row r="53" spans="1:2" ht="31.5" customHeight="1">
+    <row r="53" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="72"/>
       <c r="B53" s="70" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="51">
+    <row r="54" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="66" t="s">
         <v>136</v>
       </c>
@@ -10355,7 +10379,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="120.75" customHeight="1">
+    <row r="55" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="66" t="s">
         <v>165</v>
       </c>
@@ -10363,7 +10387,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="92.25" customHeight="1">
+    <row r="56" spans="1:2" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="66" t="s">
         <v>198</v>
       </c>
@@ -10371,7 +10395,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="17.100000000000001">
+    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="66" t="s">
         <v>233</v>
       </c>
@@ -10379,7 +10403,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="45" customHeight="1">
+    <row r="58" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="66" t="s">
         <v>256</v>
       </c>
@@ -10387,7 +10411,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="82.5" customHeight="1">
+    <row r="59" spans="1:2" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="66" t="s">
         <v>289</v>
       </c>
@@ -10395,7 +10419,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="68.099999999999994">
+    <row r="60" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A60" s="66" t="s">
         <v>328</v>
       </c>
@@ -10403,7 +10427,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="51">
+    <row r="61" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="66" t="s">
         <v>370</v>
       </c>
@@ -10411,7 +10435,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="33.950000000000003">
+    <row r="62" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="66" t="s">
         <v>413</v>
       </c>
@@ -10419,7 +10443,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="51">
+    <row r="63" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="66" t="s">
         <v>456</v>
       </c>
@@ -10427,7 +10451,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="75" customHeight="1">
+    <row r="66" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="64"/>
       <c r="B66" s="70" t="s">
         <v>129</v>
@@ -10436,7 +10460,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="63.95">
+    <row r="67" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A67" s="70" t="s">
         <v>136</v>
       </c>
@@ -10447,7 +10471,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="17.100000000000001">
+    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="70" t="s">
         <v>165</v>
       </c>
@@ -10458,7 +10482,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="17.100000000000001">
+    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="70" t="s">
         <v>198</v>
       </c>
@@ -10469,7 +10493,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="17.100000000000001">
+    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="70" t="s">
         <v>233</v>
       </c>
@@ -10480,7 +10504,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="33.950000000000003">
+    <row r="71" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="70" t="s">
         <v>256</v>
       </c>
@@ -10491,7 +10515,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="84.95">
+    <row r="72" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A72" s="70" t="s">
         <v>289</v>
       </c>
@@ -10502,7 +10526,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="17.100000000000001">
+    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="70" t="s">
         <v>328</v>
       </c>
@@ -10513,7 +10537,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="33.950000000000003">
+    <row r="74" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="70" t="s">
         <v>370</v>
       </c>
@@ -10524,7 +10548,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="68.099999999999994">
+    <row r="75" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A75" s="70" t="s">
         <v>413</v>
       </c>
@@ -10535,7 +10559,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="17.100000000000001">
+    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="70" t="s">
         <v>456</v>
       </c>
@@ -10559,21 +10583,21 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="71" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="34.5" customHeight="1">
+    <row r="2" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="72"/>
       <c r="B2" s="70" t="s">
         <v>499</v>
@@ -10588,7 +10612,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1">
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="66" t="s">
         <v>136</v>
       </c>
@@ -10603,7 +10627,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="66" t="s">
         <v>165</v>
       </c>
@@ -10620,7 +10644,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.100000000000001">
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="66" t="s">
         <v>198</v>
       </c>
@@ -10637,7 +10661,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" customHeight="1">
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="66" t="s">
         <v>233</v>
       </c>
@@ -10654,7 +10678,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.100000000000001">
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="66" t="s">
         <v>256</v>
       </c>
@@ -10671,7 +10695,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="33.950000000000003">
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="66" t="s">
         <v>289</v>
       </c>
@@ -10686,7 +10710,7 @@
       </c>
       <c r="E8" s="69"/>
     </row>
-    <row r="9" spans="1:5" ht="17.100000000000001">
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="66" t="s">
         <v>328</v>
       </c>
@@ -10703,7 +10727,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.100000000000001">
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="66" t="s">
         <v>370</v>
       </c>
@@ -10718,7 +10742,7 @@
       </c>
       <c r="E10" s="69"/>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="66" t="s">
         <v>413</v>
       </c>
@@ -10733,7 +10757,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="27" customHeight="1">
+    <row r="12" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="66" t="s">
         <v>456</v>
       </c>
@@ -10750,7 +10774,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="51">
+    <row r="15" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="72"/>
       <c r="B15" s="70" t="s">
         <v>102</v>
@@ -10759,7 +10783,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17.100000000000001">
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="66" t="s">
         <v>136</v>
       </c>
@@ -10768,7 +10792,7 @@
       </c>
       <c r="C16" s="66"/>
     </row>
-    <row r="17" spans="1:3" ht="17.100000000000001">
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="66" t="s">
         <v>165</v>
       </c>
@@ -10779,7 +10803,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.100000000000001">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="66" t="s">
         <v>198</v>
       </c>
@@ -10790,7 +10814,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.100000000000001">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="66" t="s">
         <v>233</v>
       </c>
@@ -10801,7 +10825,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.100000000000001">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="66" t="s">
         <v>256</v>
       </c>
@@ -10812,7 +10836,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33.950000000000003">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="66" t="s">
         <v>289</v>
       </c>
@@ -10823,7 +10847,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="33.950000000000003">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="66" t="s">
         <v>328</v>
       </c>
@@ -10834,7 +10858,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="51">
+    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="66" t="s">
         <v>370</v>
       </c>
@@ -10845,7 +10869,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="68.099999999999994">
+    <row r="24" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="66" t="s">
         <v>413</v>
       </c>
@@ -10856,7 +10880,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="33.950000000000003">
+    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="66" t="s">
         <v>456</v>
       </c>
@@ -10867,19 +10891,19 @@
         <v>482</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="51">
+    <row r="28" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="72"/>
       <c r="B28" s="70" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17.100000000000001">
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="66" t="s">
         <v>136</v>
       </c>
       <c r="B29" s="66"/>
     </row>
-    <row r="30" spans="1:3" ht="17.100000000000001">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="66" t="s">
         <v>165</v>
       </c>
@@ -10887,7 +10911,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17.100000000000001">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="66" t="s">
         <v>198</v>
       </c>
@@ -10895,7 +10919,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="51">
+    <row r="32" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="66" t="s">
         <v>233</v>
       </c>
@@ -10903,7 +10927,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="17.100000000000001">
+    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="66" t="s">
         <v>256</v>
       </c>
@@ -10911,7 +10935,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17.100000000000001">
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="66" t="s">
         <v>289</v>
       </c>
@@ -10919,7 +10943,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17.100000000000001">
+    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="66" t="s">
         <v>328</v>
       </c>
@@ -10927,13 +10951,13 @@
         <v>356</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17.100000000000001">
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="66" t="s">
         <v>370</v>
       </c>
       <c r="B36" s="66"/>
     </row>
-    <row r="37" spans="1:2" ht="17.100000000000001">
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="74" t="s">
         <v>413</v>
       </c>
@@ -10941,7 +10965,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="33.950000000000003">
+    <row r="38" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="66" t="s">
         <v>456</v>
       </c>
@@ -10949,29 +10973,29 @@
         <v>545</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.95">
+    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="62"/>
       <c r="B39" s="62"/>
     </row>
-    <row r="40" spans="1:2" ht="33.950000000000003">
+    <row r="40" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="72"/>
       <c r="B40" s="70" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17.100000000000001">
+    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="66" t="s">
         <v>136</v>
       </c>
       <c r="B41" s="66"/>
     </row>
-    <row r="42" spans="1:2" ht="17.100000000000001">
+    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="66" t="s">
         <v>165</v>
       </c>
       <c r="B42" s="66"/>
     </row>
-    <row r="43" spans="1:2" ht="17.100000000000001">
+    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="66" t="s">
         <v>198</v>
       </c>
@@ -10979,7 +11003,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17.100000000000001">
+    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="66" t="s">
         <v>233</v>
       </c>
@@ -10987,7 +11011,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="33.950000000000003">
+    <row r="45" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="66" t="s">
         <v>256</v>
       </c>
@@ -10995,13 +11019,13 @@
         <v>278</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17.100000000000001">
+    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="66" t="s">
         <v>289</v>
       </c>
       <c r="B46" s="66"/>
     </row>
-    <row r="47" spans="1:2" ht="33.950000000000003">
+    <row r="47" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="66" t="s">
         <v>328</v>
       </c>
@@ -11009,7 +11033,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="33.950000000000003">
+    <row r="48" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="66" t="s">
         <v>370</v>
       </c>
@@ -11017,7 +11041,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="17.100000000000001">
+    <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="66" t="s">
         <v>413</v>
       </c>
@@ -11025,7 +11049,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="17.100000000000001">
+    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="66" t="s">
         <v>456</v>
       </c>
@@ -11033,7 +11057,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.95">
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="62"/>
     </row>
   </sheetData>
@@ -11049,20 +11073,20 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" style="51" customWidth="1"/>
-    <col min="2" max="2" width="109.42578125" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" customWidth="1"/>
-    <col min="4" max="4" width="64.140625" customWidth="1"/>
+    <col min="2" max="2" width="109.5" customWidth="1"/>
+    <col min="3" max="3" width="56.1640625" customWidth="1"/>
+    <col min="4" max="4" width="64.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="71" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="63"/>
       <c r="B3" s="70" t="s">
         <v>546</v>
@@ -11074,7 +11098,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.100000000000001">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="65" t="s">
         <v>136</v>
       </c>
@@ -11088,7 +11112,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.100000000000001">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="65" t="s">
         <v>165</v>
       </c>
@@ -11100,7 +11124,7 @@
       </c>
       <c r="D5" s="69"/>
     </row>
-    <row r="6" spans="1:4" ht="17.100000000000001">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="67" t="s">
         <v>198</v>
       </c>
@@ -11112,7 +11136,7 @@
       </c>
       <c r="D6" s="69"/>
     </row>
-    <row r="7" spans="1:4" ht="17.100000000000001">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="68" t="s">
         <v>233</v>
       </c>
@@ -11124,7 +11148,7 @@
       </c>
       <c r="D7" s="69"/>
     </row>
-    <row r="8" spans="1:4" ht="51">
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="67" t="s">
         <v>256</v>
       </c>
@@ -11136,7 +11160,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.100000000000001">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="68" t="s">
         <v>289</v>
       </c>
@@ -11150,7 +11174,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="33.950000000000003">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="67" t="s">
         <v>328</v>
       </c>
@@ -11162,7 +11186,7 @@
       </c>
       <c r="D10" s="69"/>
     </row>
-    <row r="11" spans="1:4" ht="33.950000000000003">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="68" t="s">
         <v>370</v>
       </c>
@@ -11174,7 +11198,7 @@
       </c>
       <c r="D11" s="69"/>
     </row>
-    <row r="12" spans="1:4" ht="17.100000000000001">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="67" t="s">
         <v>413</v>
       </c>
@@ -11188,7 +11212,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.100000000000001">
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="68" t="s">
         <v>456</v>
       </c>
@@ -11200,13 +11224,13 @@
       </c>
       <c r="D13" s="69"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="63"/>
       <c r="B19" s="64" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="33.950000000000003">
+    <row r="20" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="65" t="s">
         <v>136</v>
       </c>
@@ -11214,7 +11238,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1">
+    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="65" t="s">
         <v>165</v>
       </c>
@@ -11222,7 +11246,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17.100000000000001">
+    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="67" t="s">
         <v>198</v>
       </c>
@@ -11230,7 +11254,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="17.100000000000001">
+    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="68" t="s">
         <v>233</v>
       </c>
@@ -11238,7 +11262,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="33.950000000000003">
+    <row r="24" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="67" t="s">
         <v>256</v>
       </c>
@@ -11246,13 +11270,13 @@
         <v>549</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.95">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="68" t="s">
         <v>289</v>
       </c>
       <c r="B25" s="66"/>
     </row>
-    <row r="26" spans="1:2" ht="33.950000000000003">
+    <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="67" t="s">
         <v>328</v>
       </c>
@@ -11260,7 +11284,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="51">
+    <row r="27" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="68" t="s">
         <v>370</v>
       </c>
@@ -11268,7 +11292,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17.100000000000001">
+    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="67" t="s">
         <v>413</v>
       </c>
@@ -11276,25 +11300,25 @@
         <v>453</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.95">
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="68" t="s">
         <v>456</v>
       </c>
       <c r="B29" s="66"/>
     </row>
-    <row r="34" spans="1:2" ht="33.950000000000003">
+    <row r="34" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="63"/>
       <c r="B34" s="70" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.95">
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="65" t="s">
         <v>136</v>
       </c>
       <c r="B35" s="66"/>
     </row>
-    <row r="36" spans="1:2" ht="17.100000000000001">
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="65" t="s">
         <v>165</v>
       </c>
@@ -11302,7 +11326,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17.100000000000001">
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="67" t="s">
         <v>198</v>
       </c>
@@ -11310,7 +11334,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17.100000000000001">
+    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="68" t="s">
         <v>233</v>
       </c>
@@ -11318,7 +11342,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="33.950000000000003">
+    <row r="39" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="67" t="s">
         <v>256</v>
       </c>
@@ -11326,7 +11350,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17.100000000000001">
+    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="68" t="s">
         <v>289</v>
       </c>
@@ -11334,7 +11358,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17.100000000000001">
+    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="67" t="s">
         <v>328</v>
       </c>
@@ -11342,7 +11366,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17.100000000000001">
+    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="68" t="s">
         <v>370</v>
       </c>
@@ -11350,7 +11374,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="33.950000000000003">
+    <row r="43" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="67" t="s">
         <v>413</v>
       </c>
@@ -11358,7 +11382,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17.100000000000001">
+    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="68" t="s">
         <v>456</v>
       </c>
@@ -11379,16 +11403,16 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="57.42578125" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="57.5" customWidth="1"/>
+    <col min="3" max="3" width="75.5" customWidth="1"/>
     <col min="4" max="4" width="56" customWidth="1"/>
-    <col min="5" max="5" width="88.42578125" customWidth="1"/>
+    <col min="5" max="5" width="88.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="81" customFormat="1" ht="32.1">
+    <row r="1" spans="1:5" s="81" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="82"/>
       <c r="B1" s="83" t="s">
         <v>554</v>
@@ -11403,7 +11427,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.95">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="84" t="s">
         <v>136</v>
       </c>
@@ -11412,7 +11436,7 @@
       <c r="D2" s="84"/>
       <c r="E2" s="84"/>
     </row>
-    <row r="3" spans="1:5" ht="15.95">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="65" t="s">
         <v>165</v>
       </c>
@@ -11421,7 +11445,7 @@
       <c r="D3" s="65"/>
       <c r="E3" s="65"/>
     </row>
-    <row r="4" spans="1:5" ht="15.95">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="67" t="s">
         <v>198</v>
       </c>
@@ -11430,7 +11454,7 @@
       <c r="D4" s="67"/>
       <c r="E4" s="67"/>
     </row>
-    <row r="5" spans="1:5" ht="15.95">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="68" t="s">
         <v>233</v>
       </c>
@@ -11439,7 +11463,7 @@
       <c r="D5" s="68"/>
       <c r="E5" s="68"/>
     </row>
-    <row r="6" spans="1:5" ht="96" customHeight="1">
+    <row r="6" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="67" t="s">
         <v>256</v>
       </c>
@@ -11454,7 +11478,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.95">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="68" t="s">
         <v>289</v>
       </c>
@@ -11465,7 +11489,7 @@
       <c r="D7" s="68"/>
       <c r="E7" s="68"/>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="67" t="s">
         <v>328</v>
       </c>
@@ -11476,7 +11500,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.95">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="68" t="s">
         <v>370</v>
       </c>
@@ -11487,7 +11511,7 @@
       <c r="D9" s="68"/>
       <c r="E9" s="68"/>
     </row>
-    <row r="10" spans="1:5" ht="15.95">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="67" t="s">
         <v>413</v>
       </c>
@@ -11498,7 +11522,7 @@
       <c r="D10" s="67"/>
       <c r="E10" s="67"/>
     </row>
-    <row r="11" spans="1:5" ht="15.95">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="68" t="s">
         <v>456</v>
       </c>
@@ -11522,15 +11546,15 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1">
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="98" t="s">
         <v>64</v>
       </c>
@@ -11544,7 +11568,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1">
+    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="88" t="s">
         <v>136</v>
       </c>
@@ -11556,7 +11580,7 @@
       </c>
       <c r="D2" s="89"/>
     </row>
-    <row r="3" spans="1:4" ht="30.75" customHeight="1">
+    <row r="3" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="90" t="s">
         <v>165</v>
       </c>
@@ -11570,7 +11594,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.95">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="92" t="s">
         <v>198</v>
       </c>
@@ -11582,7 +11606,7 @@
       </c>
       <c r="D4" s="93"/>
     </row>
-    <row r="5" spans="1:4" ht="15.95">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="94" t="s">
         <v>233</v>
       </c>
@@ -11594,7 +11618,7 @@
       </c>
       <c r="D5" s="95"/>
     </row>
-    <row r="6" spans="1:4" ht="15.95">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="92" t="s">
         <v>256</v>
       </c>
@@ -11606,7 +11630,7 @@
       </c>
       <c r="D6" s="93"/>
     </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1">
+    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="94" t="s">
         <v>289</v>
       </c>
@@ -11618,7 +11642,7 @@
       </c>
       <c r="D7" s="95"/>
     </row>
-    <row r="8" spans="1:4" ht="15.95">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="92" t="s">
         <v>328</v>
       </c>
@@ -11630,7 +11654,7 @@
       </c>
       <c r="D8" s="93"/>
     </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1">
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="94" t="s">
         <v>370</v>
       </c>
@@ -11642,7 +11666,7 @@
       </c>
       <c r="D9" s="95"/>
     </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1">
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="92" t="s">
         <v>413</v>
       </c>
@@ -11654,7 +11678,7 @@
       </c>
       <c r="D10" s="93"/>
     </row>
-    <row r="11" spans="1:4" ht="30" customHeight="1">
+    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="96" t="s">
         <v>456</v>
       </c>
@@ -11675,38 +11699,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B81DAE-D652-4BB6-8C73-F96210539325}">
   <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M3" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="120.7109375" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="60.7109375" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="70.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="80.7109375" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" customWidth="1"/>
-    <col min="20" max="20" width="30.7109375" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" customWidth="1"/>
-    <col min="23" max="23" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="120.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="60.6640625" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="70.6640625" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="80.6640625" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" customWidth="1"/>
+    <col min="20" max="20" width="30.6640625" customWidth="1"/>
+    <col min="21" max="21" width="6.6640625" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" customWidth="1"/>
+    <col min="23" max="23" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45" customHeight="1">
+    <row r="1" spans="1:17" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="123" t="s">
         <v>560</v>
       </c>
@@ -11744,7 +11768,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="168.75" customHeight="1">
+    <row r="2" spans="1:17" ht="168.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="113" t="s">
         <v>136</v>
       </c>
@@ -11785,7 +11809,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="86.25" customHeight="1">
+    <row r="3" spans="1:17" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="114" t="s">
         <v>165</v>
       </c>
@@ -11828,7 +11852,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="36" customHeight="1">
+    <row r="4" spans="1:17" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="115" t="s">
         <v>198</v>
       </c>
@@ -11871,7 +11895,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="37.5" customHeight="1">
+    <row r="5" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="116" t="s">
         <v>233</v>
       </c>
@@ -11912,7 +11936,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="34.5" customHeight="1">
+    <row r="6" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115" t="s">
         <v>256</v>
       </c>
@@ -11955,7 +11979,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="75.75" customHeight="1">
+    <row r="7" spans="1:17" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="116" t="s">
         <v>289</v>
       </c>
@@ -11998,7 +12022,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="116.25" customHeight="1">
+    <row r="8" spans="1:17" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115" t="s">
         <v>328</v>
       </c>
@@ -12041,7 +12065,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="51.75" customHeight="1">
+    <row r="9" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="116" t="s">
         <v>370</v>
       </c>
@@ -12084,7 +12108,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="33.75" customHeight="1">
+    <row r="10" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="115" t="s">
         <v>413</v>
       </c>
@@ -12127,7 +12151,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="48" customHeight="1">
+    <row r="11" spans="1:17" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="117" t="s">
         <v>456</v>
       </c>
@@ -12170,7 +12194,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="48">
+    <row r="13" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="126" t="s">
         <v>567</v>
       </c>
@@ -12193,7 +12217,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="111.95">
+    <row r="14" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A14" s="113" t="s">
         <v>136</v>
       </c>
@@ -12220,7 +12244,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="80.099999999999994">
+    <row r="15" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="114" t="s">
         <v>165</v>
       </c>
@@ -12246,7 +12270,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="80.099999999999994">
+    <row r="16" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="115" t="s">
         <v>198</v>
       </c>
@@ -12272,7 +12296,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15.95">
+    <row r="17" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="116" t="s">
         <v>233</v>
       </c>
@@ -12296,7 +12320,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="32.1">
+    <row r="18" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="115" t="s">
         <v>256</v>
       </c>
@@ -12322,7 +12346,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="75">
+    <row r="19" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A19" s="116" t="s">
         <v>289</v>
       </c>
@@ -12348,7 +12372,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="80.099999999999994">
+    <row r="20" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" s="115" t="s">
         <v>328</v>
       </c>
@@ -12374,7 +12398,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="48">
+    <row r="21" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="116" t="s">
         <v>370</v>
       </c>
@@ -12400,7 +12424,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="105">
+    <row r="22" spans="1:23" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="115" t="s">
         <v>413</v>
       </c>
@@ -12426,7 +12450,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="32.1">
+    <row r="23" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="117" t="s">
         <v>456</v>
       </c>
@@ -12450,7 +12474,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="25" spans="1:23" s="152" customFormat="1" ht="75">
+    <row r="25" spans="1:23" s="152" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A25" s="150" t="s">
         <v>571</v>
       </c>
@@ -12501,7 +12525,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="32.1">
+    <row r="26" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="113" t="s">
         <v>136</v>
       </c>
@@ -12549,7 +12573,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="322.5" customHeight="1">
+    <row r="27" spans="1:23" ht="322.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="114" t="s">
         <v>165</v>
       </c>
@@ -12599,7 +12623,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="80.25" customHeight="1">
+    <row r="28" spans="1:23" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="115" t="s">
         <v>198</v>
       </c>
@@ -12649,7 +12673,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="48">
+    <row r="29" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="116" t="s">
         <v>233</v>
       </c>
@@ -12699,7 +12723,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="51" customHeight="1">
+    <row r="30" spans="1:23" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="115" t="s">
         <v>256</v>
       </c>
@@ -12747,7 +12771,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="126.75" customHeight="1">
+    <row r="31" spans="1:23" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="116" t="s">
         <v>289</v>
       </c>
@@ -12797,7 +12821,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="63.95">
+    <row r="32" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A32" s="115" t="s">
         <v>328</v>
       </c>
@@ -12847,7 +12871,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="66" customHeight="1">
+    <row r="33" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="116" t="s">
         <v>370</v>
       </c>
@@ -12897,7 +12921,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="45">
+    <row r="34" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="115" t="s">
         <v>413</v>
       </c>
@@ -12943,7 +12967,7 @@
       </c>
       <c r="W34" s="103"/>
     </row>
-    <row r="35" spans="1:23" ht="63.95">
+    <row r="35" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" s="117" t="s">
         <v>456</v>
       </c>
@@ -12991,7 +13015,7 @@
       </c>
       <c r="W35" s="105"/>
     </row>
-    <row r="37" spans="1:23" s="152" customFormat="1" ht="105">
+    <row r="37" spans="1:23" s="152" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A37" s="150" t="s">
         <v>581</v>
       </c>
@@ -13041,7 +13065,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="48">
+    <row r="38" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="113" t="s">
         <v>136</v>
       </c>
@@ -13087,7 +13111,7 @@
       </c>
       <c r="W38" s="111"/>
     </row>
-    <row r="39" spans="1:23" ht="111.95">
+    <row r="39" spans="1:23" ht="112" x14ac:dyDescent="0.2">
       <c r="A39" s="114" t="s">
         <v>165</v>
       </c>
@@ -13137,7 +13161,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="111.95">
+    <row r="40" spans="1:23" ht="112" x14ac:dyDescent="0.2">
       <c r="A40" s="115" t="s">
         <v>198</v>
       </c>
@@ -13187,7 +13211,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="32.1">
+    <row r="41" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="116" t="s">
         <v>233</v>
       </c>
@@ -13237,7 +13261,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="63.95">
+    <row r="42" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" s="115" t="s">
         <v>256</v>
       </c>
@@ -13287,7 +13311,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="135">
+    <row r="43" spans="1:23" ht="144" x14ac:dyDescent="0.2">
       <c r="A43" s="116" t="s">
         <v>289</v>
       </c>
@@ -13337,7 +13361,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="80.099999999999994">
+    <row r="44" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A44" s="115" t="s">
         <v>328</v>
       </c>
@@ -13387,7 +13411,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="66" customHeight="1">
+    <row r="45" spans="1:23" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="116" t="s">
         <v>370</v>
       </c>
@@ -13437,7 +13461,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="75">
+    <row r="46" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A46" s="115" t="s">
         <v>413</v>
       </c>
@@ -13487,7 +13511,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="111" customHeight="1">
+    <row r="47" spans="1:23" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="117" t="s">
         <v>456</v>
       </c>
@@ -13533,7 +13557,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="48">
+    <row r="49" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" s="129" t="s">
         <v>589</v>
       </c>
@@ -13541,31 +13565,31 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.95">
+    <row r="50" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="113" t="s">
         <v>136</v>
       </c>
       <c r="B50" s="111"/>
     </row>
-    <row r="51" spans="1:2" ht="15.95">
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="114" t="s">
         <v>165</v>
       </c>
       <c r="B51" s="102"/>
     </row>
-    <row r="52" spans="1:2" ht="15.95">
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="115" t="s">
         <v>198</v>
       </c>
       <c r="B52" s="103"/>
     </row>
-    <row r="53" spans="1:2" ht="15.95">
+    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="116" t="s">
         <v>233</v>
       </c>
       <c r="B53" s="104"/>
     </row>
-    <row r="54" spans="1:2" ht="15.95">
+    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="115" t="s">
         <v>256</v>
       </c>
@@ -13573,7 +13597,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.95">
+    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="116" t="s">
         <v>289</v>
       </c>
@@ -13581,13 +13605,13 @@
         <v>177</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.95">
+    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="115" t="s">
         <v>328</v>
       </c>
       <c r="B56" s="103"/>
     </row>
-    <row r="57" spans="1:2" ht="15.95">
+    <row r="57" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="116" t="s">
         <v>370</v>
       </c>
@@ -13595,13 +13619,13 @@
         <v>396</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.95">
+    <row r="58" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="115" t="s">
         <v>413</v>
       </c>
       <c r="B58" s="103"/>
     </row>
-    <row r="59" spans="1:2" ht="15.95">
+    <row r="59" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="117" t="s">
         <v>456</v>
       </c>
@@ -13616,38 +13640,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF55BB61-3A6F-4270-90C9-AB8A8506205C}">
   <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="30.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="30.7109375" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" customWidth="1"/>
-    <col min="20" max="20" width="30.7109375" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" customWidth="1"/>
-    <col min="23" max="23" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="30.6640625" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="30.6640625" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" customWidth="1"/>
+    <col min="20" max="20" width="30.6640625" customWidth="1"/>
+    <col min="21" max="21" width="6.6640625" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" customWidth="1"/>
+    <col min="23" max="23" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="80.099999999999994">
+    <row r="1" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A1" s="132" t="s">
         <v>590</v>
       </c>
@@ -13673,11 +13697,13 @@
         <v>502</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="19.5" customHeight="1">
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="113" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="111"/>
+      <c r="B2" s="103" t="s">
+        <v>274</v>
+      </c>
       <c r="D2" s="113" t="s">
         <v>136</v>
       </c>
@@ -13691,16 +13717,16 @@
       <c r="J2" s="113" t="s">
         <v>136</v>
       </c>
-      <c r="K2" s="121" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="30.75" customHeight="1">
+      <c r="K2" s="103" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="114" t="s">
         <v>165</v>
       </c>
       <c r="B3" s="102" t="s">
-        <v>190</v>
+        <v>604</v>
       </c>
       <c r="D3" s="114" t="s">
         <v>165</v>
@@ -13718,10 +13744,10 @@
         <v>165</v>
       </c>
       <c r="K3" s="102" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.95">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="115" t="s">
         <v>198</v>
       </c>
@@ -13732,7 +13758,7 @@
         <v>198</v>
       </c>
       <c r="E4" s="103" t="s">
-        <v>220</v>
+        <v>274</v>
       </c>
       <c r="G4" s="115" t="s">
         <v>198</v>
@@ -13744,10 +13770,10 @@
         <v>198</v>
       </c>
       <c r="K4" s="103" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.95">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="116" t="s">
         <v>233</v>
       </c>
@@ -13757,8 +13783,8 @@
       <c r="D5" s="116" t="s">
         <v>233</v>
       </c>
-      <c r="E5" s="104" t="s">
-        <v>220</v>
+      <c r="E5" s="103" t="s">
+        <v>274</v>
       </c>
       <c r="G5" s="116" t="s">
         <v>233</v>
@@ -13770,10 +13796,10 @@
         <v>233</v>
       </c>
       <c r="K5" s="104" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="15.95">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="115" t="s">
         <v>256</v>
       </c>
@@ -13799,131 +13825,138 @@
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="49.5" customHeight="1">
+    <row r="7" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="116" t="s">
         <v>289</v>
       </c>
       <c r="B7" s="104" t="s">
-        <v>311</v>
+        <v>600</v>
       </c>
       <c r="D7" s="116" t="s">
         <v>289</v>
       </c>
       <c r="E7" s="104" t="s">
-        <v>312</v>
+        <v>605</v>
       </c>
       <c r="G7" s="116" t="s">
         <v>289</v>
       </c>
       <c r="H7" s="104" t="s">
-        <v>313</v>
+        <v>606</v>
       </c>
       <c r="J7" s="116" t="s">
         <v>289</v>
       </c>
-      <c r="K7" s="104"/>
-    </row>
-    <row r="8" spans="1:11" ht="45.75" customHeight="1">
+      <c r="K7" s="104" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115" t="s">
         <v>328</v>
       </c>
       <c r="B8" s="103" t="s">
-        <v>349</v>
+        <v>601</v>
       </c>
       <c r="D8" s="115" t="s">
         <v>328</v>
       </c>
       <c r="E8" s="103" t="s">
-        <v>350</v>
+        <v>274</v>
       </c>
       <c r="G8" s="115" t="s">
         <v>328</v>
       </c>
       <c r="H8" s="103" t="s">
-        <v>351</v>
+        <v>608</v>
       </c>
       <c r="J8" s="115" t="s">
         <v>328</v>
       </c>
       <c r="K8" s="103" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="17.25" customHeight="1">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="116" t="s">
         <v>370</v>
       </c>
       <c r="B9" s="104" t="s">
-        <v>397</v>
+        <v>350</v>
       </c>
       <c r="D9" s="116" t="s">
         <v>370</v>
       </c>
-      <c r="E9" s="104"/>
+      <c r="E9" s="104" t="s">
+        <v>602</v>
+      </c>
       <c r="G9" s="116" t="s">
         <v>370</v>
       </c>
       <c r="H9" s="104" t="s">
-        <v>397</v>
+        <v>350</v>
       </c>
       <c r="J9" s="116" t="s">
         <v>370</v>
       </c>
       <c r="K9" s="104" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="50.25" customHeight="1">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="115" t="s">
         <v>413</v>
       </c>
       <c r="B10" s="103" t="s">
-        <v>436</v>
+        <v>274</v>
       </c>
       <c r="D10" s="115" t="s">
         <v>413</v>
       </c>
-      <c r="E10" s="103"/>
+      <c r="E10" s="103" t="s">
+        <v>274</v>
+      </c>
       <c r="G10" s="115" t="s">
         <v>413</v>
       </c>
       <c r="H10" s="103" t="s">
-        <v>437</v>
+        <v>607</v>
       </c>
       <c r="J10" s="115" t="s">
         <v>413</v>
       </c>
       <c r="K10" s="103" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="67.5" customHeight="1">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="117" t="s">
         <v>456</v>
       </c>
       <c r="B11" s="105" t="s">
-        <v>477</v>
+        <v>603</v>
       </c>
       <c r="D11" s="117" t="s">
         <v>456</v>
       </c>
       <c r="E11" s="105" t="s">
-        <v>478</v>
+        <v>274</v>
       </c>
       <c r="G11" s="117" t="s">
         <v>456</v>
       </c>
       <c r="H11" s="105" t="s">
-        <v>479</v>
+        <v>609</v>
       </c>
       <c r="J11" s="117" t="s">
         <v>456</v>
       </c>
       <c r="K11" s="105" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="63.95">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="134" t="s">
         <v>594</v>
       </c>
@@ -13949,7 +13982,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.95">
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="113" t="s">
         <v>136</v>
       </c>
@@ -13969,7 +14002,7 @@
       </c>
       <c r="K14" s="111"/>
     </row>
-    <row r="15" spans="1:11" ht="30">
+    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="114" t="s">
         <v>165</v>
       </c>
@@ -13993,7 +14026,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="32.1">
+    <row r="16" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="115" t="s">
         <v>198</v>
       </c>
@@ -14019,7 +14052,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="32.1">
+    <row r="17" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="116" t="s">
         <v>233</v>
       </c>
@@ -14045,7 +14078,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="15.95">
+    <row r="18" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="115" t="s">
         <v>256</v>
       </c>
@@ -14071,7 +14104,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="75">
+    <row r="19" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A19" s="116" t="s">
         <v>289</v>
       </c>
@@ -14097,7 +14130,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="30">
+    <row r="20" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="115" t="s">
         <v>328</v>
       </c>
@@ -14123,7 +14156,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="75">
+    <row r="21" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="116" t="s">
         <v>370</v>
       </c>
@@ -14149,7 +14182,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="180">
+    <row r="22" spans="1:23" ht="160" x14ac:dyDescent="0.2">
       <c r="A22" s="115" t="s">
         <v>413</v>
       </c>
@@ -14175,7 +14208,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="48">
+    <row r="23" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" s="117" t="s">
         <v>456</v>
       </c>
@@ -14201,7 +14234,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="101.25" customHeight="1">
+    <row r="25" spans="1:23" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="136"/>
       <c r="B25" s="140" t="s">
         <v>74</v>
@@ -14235,7 +14268,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="15.95">
+    <row r="26" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="113" t="s">
         <v>136</v>
       </c>
@@ -14269,7 +14302,7 @@
       </c>
       <c r="W26" s="137"/>
     </row>
-    <row r="27" spans="1:23" ht="17.100000000000001">
+    <row r="27" spans="1:23" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="114" t="s">
         <v>165</v>
       </c>
@@ -14305,7 +14338,7 @@
       </c>
       <c r="W27" s="102"/>
     </row>
-    <row r="28" spans="1:23" ht="60">
+    <row r="28" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="115" t="s">
         <v>198</v>
       </c>
@@ -14355,7 +14388,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="111.95">
+    <row r="29" spans="1:23" ht="112" x14ac:dyDescent="0.2">
       <c r="A29" s="116" t="s">
         <v>233</v>
       </c>
@@ -14405,7 +14438,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="63.95">
+    <row r="30" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="115" t="s">
         <v>256</v>
       </c>
@@ -14455,7 +14488,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="150">
+    <row r="31" spans="1:23" ht="144" x14ac:dyDescent="0.2">
       <c r="A31" s="116" t="s">
         <v>289</v>
       </c>
@@ -14499,7 +14532,7 @@
       </c>
       <c r="W31" s="104"/>
     </row>
-    <row r="32" spans="1:23" ht="96">
+    <row r="32" spans="1:23" ht="96" x14ac:dyDescent="0.2">
       <c r="A32" s="115" t="s">
         <v>328</v>
       </c>
@@ -14549,7 +14582,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="45">
+    <row r="33" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="116" t="s">
         <v>370</v>
       </c>
@@ -14599,7 +14632,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="105">
+    <row r="34" spans="1:23" ht="96" x14ac:dyDescent="0.2">
       <c r="A34" s="115" t="s">
         <v>413</v>
       </c>
@@ -14649,7 +14682,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="80.099999999999994">
+    <row r="35" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A35" s="117" t="s">
         <v>456</v>
       </c>
@@ -14699,7 +14732,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="48">
+    <row r="37" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="141"/>
       <c r="B37" s="143" t="s">
         <v>82</v>
@@ -14709,7 +14742,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="15.95">
+    <row r="38" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="113" t="s">
         <v>136</v>
       </c>
@@ -14719,7 +14752,7 @@
       </c>
       <c r="E38" s="137"/>
     </row>
-    <row r="39" spans="1:23" ht="15.95">
+    <row r="39" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="114" t="s">
         <v>165</v>
       </c>
@@ -14731,7 +14764,7 @@
       </c>
       <c r="E39" s="102"/>
     </row>
-    <row r="40" spans="1:23" ht="15.95">
+    <row r="40" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="115" t="s">
         <v>198</v>
       </c>
@@ -14743,7 +14776,7 @@
       </c>
       <c r="E40" s="103"/>
     </row>
-    <row r="41" spans="1:23" ht="15.95">
+    <row r="41" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="116" t="s">
         <v>233</v>
       </c>
@@ -14755,7 +14788,7 @@
       </c>
       <c r="E41" s="104"/>
     </row>
-    <row r="42" spans="1:23" ht="207.95">
+    <row r="42" spans="1:23" ht="208" x14ac:dyDescent="0.2">
       <c r="A42" s="115" t="s">
         <v>256</v>
       </c>
@@ -14769,7 +14802,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="96">
+    <row r="43" spans="1:23" ht="96" x14ac:dyDescent="0.2">
       <c r="A43" s="116" t="s">
         <v>289</v>
       </c>
@@ -14781,7 +14814,7 @@
       </c>
       <c r="E43" s="104"/>
     </row>
-    <row r="44" spans="1:23" ht="32.1">
+    <row r="44" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="115" t="s">
         <v>328</v>
       </c>
@@ -14793,7 +14826,7 @@
       </c>
       <c r="E44" s="103"/>
     </row>
-    <row r="45" spans="1:23" ht="32.1">
+    <row r="45" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="116" t="s">
         <v>370</v>
       </c>
@@ -14805,7 +14838,7 @@
       </c>
       <c r="E45" s="104"/>
     </row>
-    <row r="46" spans="1:23" ht="15.95">
+    <row r="46" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="115" t="s">
         <v>413</v>
       </c>
@@ -14819,7 +14852,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="15.95">
+    <row r="47" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="117" t="s">
         <v>456</v>
       </c>
@@ -14840,21 +14873,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A444E4101166CB49B259A75BDE06F3BF" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1da9179d651506a4ee704055c7c7620">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b3e41e30-95eb-45b9-b657-d2eda7f0eaf6" xmlns:ns3="d6ffb985-a7ae-40c0-906d-05d0dcf51054" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="22336762794d641df60944ca434000c5" ns2:_="" ns3:_="">
     <xsd:import namespace="b3e41e30-95eb-45b9-b657-d2eda7f0eaf6"/>
@@ -15065,14 +15083,53 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B45268-2425-47D2-956B-0CCF1D385955}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D05AB7-5B37-4680-A3C6-E19CC68A6CA4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b3e41e30-95eb-45b9-b657-d2eda7f0eaf6"/>
+    <ds:schemaRef ds:uri="d6ffb985-a7ae-40c0-906d-05d0dcf51054"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1918471B-3575-494A-A238-97D47571C991}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1918471B-3575-494A-A238-97D47571C991}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D05AB7-5B37-4680-A3C6-E19CC68A6CA4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B45268-2425-47D2-956B-0CCF1D385955}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
merged with DMP Annex 1, col F and G
</commit_message>
<xml_diff>
--- a/Survey.xlsx
+++ b/Survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe/Documents/GitHub/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D0A178-A7CA-1440-896B-20125A47A610}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9FF92A-059E-7F47-A86E-863AC2C8B325}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="460" windowWidth="32020" windowHeight="12460" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="32020" windowHeight="19600" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3013" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3013" uniqueCount="614">
   <si>
     <t>Colonne1</t>
   </si>
@@ -2034,32 +2034,43 @@
     <t>XML, RDF, MAG and other formats</t>
   </si>
   <si>
-    <t>TXT, MIDI</t>
-  </si>
-  <si>
     <t>MEI, MusicXML</t>
   </si>
   <si>
-    <t>CSC</t>
-  </si>
-  <si>
-    <t>RDF, Turtle</t>
-  </si>
-  <si>
     <t>ArCo, Unimarc</t>
   </si>
   <si>
-    <t>JPEG, TIFF, XML, RDF, various sound formats</t>
-  </si>
-  <si>
     <t>DOC, DOCX, WP5</t>
   </si>
   <si>
-    <t>TAR, GZIP, RDF, N-triples, RDF, RDFS, OWL</t>
-  </si>
-  <si>
-    <t>KERN, MIDI, PDF, PNG, JPG, TXT, Lilypond, MP3, HUMDRUM
-See: http://www.liederenbank.nl/mtc/</t>
+    <t>TXT, MIDI, Filemaker, CSV, XML</t>
+  </si>
+  <si>
+    <t>CSV, Filemaker, XML, TXT, HTML</t>
+  </si>
+  <si>
+    <t>RDF, Turtle, Filemaker, CSV</t>
+  </si>
+  <si>
+    <t>JPEG, TIFF, XML, RDF, HTML, various sound formats</t>
+  </si>
+  <si>
+    <t>MIDI, LY, PNG, PDF</t>
+  </si>
+  <si>
+    <t>MusicXML, MEI, MARC-XML, Essen associative code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KERN, MIDI, PDF, PNG, JPG, TXT, LY, MP3, HUMDRUM, Filemaker, JSON, HTML, ABC </t>
+  </si>
+  <si>
+    <t>TAR, GZIP, RDF, N-triples, RDF, RDFS, OWL, Filemaker, KERN, MIDI, PDF, TXT, LY, JSON, PNG</t>
+  </si>
+  <si>
+    <t>MusicXML, MEI,  MARC-XML</t>
+  </si>
+  <si>
+    <t>XML, LY, PNG, PDF, Filemaker, KERN, MIDI, PDF, TXT, JSON</t>
   </si>
 </sst>
 </file>
@@ -13641,12 +13652,12 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
@@ -13726,7 +13737,7 @@
         <v>165</v>
       </c>
       <c r="B3" s="102" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="D3" s="114" t="s">
         <v>165</v>
@@ -13738,13 +13749,13 @@
         <v>165</v>
       </c>
       <c r="H3" s="102" t="s">
-        <v>192</v>
+        <v>613</v>
       </c>
       <c r="J3" s="114" t="s">
         <v>165</v>
       </c>
       <c r="K3" s="102" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -13836,13 +13847,13 @@
         <v>289</v>
       </c>
       <c r="E7" s="104" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="G7" s="116" t="s">
         <v>289</v>
       </c>
       <c r="H7" s="104" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="J7" s="116" t="s">
         <v>289</v>
@@ -13856,7 +13867,7 @@
         <v>328</v>
       </c>
       <c r="B8" s="103" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="D8" s="115" t="s">
         <v>328</v>
@@ -13868,13 +13879,13 @@
         <v>328</v>
       </c>
       <c r="H8" s="103" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="J8" s="115" t="s">
         <v>328</v>
       </c>
       <c r="K8" s="103" t="s">
-        <v>274</v>
+        <v>612</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13888,19 +13899,19 @@
         <v>370</v>
       </c>
       <c r="E9" s="104" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="G9" s="116" t="s">
         <v>370</v>
       </c>
       <c r="H9" s="104" t="s">
-        <v>350</v>
+        <v>608</v>
       </c>
       <c r="J9" s="116" t="s">
         <v>370</v>
       </c>
       <c r="K9" s="104" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13920,7 +13931,7 @@
         <v>413</v>
       </c>
       <c r="H10" s="103" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="J10" s="115" t="s">
         <v>413</v>
@@ -13934,7 +13945,7 @@
         <v>456</v>
       </c>
       <c r="B11" s="105" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="D11" s="117" t="s">
         <v>456</v>
@@ -13946,13 +13957,13 @@
         <v>456</v>
       </c>
       <c r="H11" s="105" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="J11" s="117" t="s">
         <v>456</v>
       </c>
       <c r="K11" s="105" t="s">
-        <v>274</v>
+        <v>609</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
objective questions and validation questions updated
</commit_message>
<xml_diff>
--- a/Survey.xlsx
+++ b/Survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe/Documents/GitHub/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22B5D1BB-4B70-4A51-B877-AC5210081AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05C0094-DF20-E44D-9D59-35AC25ED9B96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="2000" windowWidth="32020" windowHeight="16460" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1680" windowWidth="32020" windowHeight="16460" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -25,27 +25,17 @@
     <sheet name="ENGAGEMENT AND VALIDATION PART" sheetId="10" r:id="rId10"/>
     <sheet name="OTHER" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3340" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3342" uniqueCount="948">
   <si>
     <t>Colonne1</t>
   </si>
@@ -3367,12 +3357,15 @@
   <si>
     <t>none yet</t>
   </si>
+  <si>
+    <t>How does the pilot relate to the stakeholder network?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="29">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3568,18 +3561,19 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="29">
@@ -5631,12 +5625,12 @@
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="35" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="35" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="35" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="7" customFormat="1" ht="80.099999999999994" hidden="1">
+    <row r="1" spans="1:61" s="7" customFormat="1" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
@@ -5809,7 +5803,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:61" s="27" customFormat="1" ht="29.25" customHeight="1">
+    <row r="2" spans="1:61" s="27" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
         <v>57</v>
       </c>
@@ -5989,7 +5983,7 @@
       </c>
       <c r="BH2" s="26"/>
     </row>
-    <row r="3" spans="1:61" s="25" customFormat="1" ht="93" customHeight="1">
+    <row r="3" spans="1:61" s="25" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>63</v>
       </c>
@@ -6168,7 +6162,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:61" s="25" customFormat="1" ht="80.099999999999994">
+    <row r="4" spans="1:61" s="25" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>90</v>
       </c>
@@ -6313,7 +6307,7 @@
       <c r="BF4" s="22"/>
       <c r="BG4" s="29"/>
     </row>
-    <row r="5" spans="1:61" s="25" customFormat="1" ht="159.94999999999999">
+    <row r="5" spans="1:61" s="25" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>109</v>
       </c>
@@ -6438,7 +6432,7 @@
       <c r="BF5" s="22"/>
       <c r="BG5" s="29"/>
     </row>
-    <row r="6" spans="1:61" s="25" customFormat="1" ht="128.1">
+    <row r="6" spans="1:61" s="25" customFormat="1" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>125</v>
       </c>
@@ -6551,7 +6545,7 @@
       <c r="BF6" s="22"/>
       <c r="BG6" s="29"/>
     </row>
-    <row r="7" spans="1:61" ht="320.10000000000002">
+    <row r="7" spans="1:61" ht="320" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>136</v>
       </c>
@@ -6653,7 +6647,7 @@
       <c r="BC7" s="36"/>
       <c r="BD7" s="36"/>
     </row>
-    <row r="8" spans="1:61" ht="15.95">
+    <row r="8" spans="1:61" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
         <v>165</v>
       </c>
@@ -6670,7 +6664,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="9" spans="1:61" ht="80.099999999999994">
+    <row r="9" spans="1:61" ht="80" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>165</v>
       </c>
@@ -6762,7 +6756,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:61" ht="15.95">
+    <row r="10" spans="1:61" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>165</v>
       </c>
@@ -6800,7 +6794,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:61" ht="176.1">
+    <row r="11" spans="1:61" ht="176" x14ac:dyDescent="0.2">
       <c r="B11" s="41" t="s">
         <v>198</v>
       </c>
@@ -6963,7 +6957,7 @@
       <c r="BG11" s="42"/>
       <c r="BH11" s="35"/>
     </row>
-    <row r="12" spans="1:61" ht="96">
+    <row r="12" spans="1:61" ht="96" x14ac:dyDescent="0.2">
       <c r="B12" s="34" t="s">
         <v>233</v>
       </c>
@@ -7122,7 +7116,7 @@
       <c r="BG12" s="43"/>
       <c r="BH12" s="46"/>
     </row>
-    <row r="13" spans="1:61" ht="176.1">
+    <row r="13" spans="1:61" ht="176" x14ac:dyDescent="0.2">
       <c r="B13" s="41" t="s">
         <v>256</v>
       </c>
@@ -7294,7 +7288,7 @@
       <c r="BH13" s="46"/>
       <c r="BI13" s="46"/>
     </row>
-    <row r="14" spans="1:61" ht="409.6">
+    <row r="14" spans="1:61" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B14" s="34" t="s">
         <v>289</v>
       </c>
@@ -7451,7 +7445,7 @@
       <c r="BG14" s="43"/>
       <c r="BH14" s="35"/>
     </row>
-    <row r="15" spans="1:61" ht="192">
+    <row r="15" spans="1:61" ht="192" x14ac:dyDescent="0.2">
       <c r="B15" s="41" t="s">
         <v>328</v>
       </c>
@@ -7616,7 +7610,7 @@
       </c>
       <c r="BH15" s="35"/>
     </row>
-    <row r="16" spans="1:61" ht="128.1">
+    <row r="16" spans="1:61" ht="128" x14ac:dyDescent="0.2">
       <c r="B16" s="34" t="s">
         <v>370</v>
       </c>
@@ -7779,7 +7773,7 @@
       <c r="BG16" s="43"/>
       <c r="BH16" s="35"/>
     </row>
-    <row r="17" spans="2:62" ht="176.1">
+    <row r="17" spans="2:62" ht="176" x14ac:dyDescent="0.2">
       <c r="B17" s="41" t="s">
         <v>413</v>
       </c>
@@ -7942,7 +7936,7 @@
       <c r="BG17" s="42"/>
       <c r="BH17" s="35"/>
     </row>
-    <row r="18" spans="2:62" ht="111.95">
+    <row r="18" spans="2:62" ht="112" x14ac:dyDescent="0.2">
       <c r="B18" s="34" t="s">
         <v>456</v>
       </c>
@@ -8111,35 +8105,37 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF88C43-E44F-455D-AEE2-5CECD1ADC60A}">
-  <dimension ref="A1:T49"/>
+  <dimension ref="A1:W49"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="111" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="N8" zoomScale="111" workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="45" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="72.140625" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="51.140625" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" customWidth="1"/>
-    <col min="16" max="16" width="17.42578125" customWidth="1"/>
-    <col min="17" max="17" width="43.140625" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" customWidth="1"/>
-    <col min="20" max="20" width="47.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="72.1640625" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
+    <col min="11" max="11" width="51.1640625" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="39.5" customWidth="1"/>
+    <col min="16" max="16" width="17.5" customWidth="1"/>
+    <col min="17" max="17" width="43.1640625" customWidth="1"/>
+    <col min="19" max="19" width="19.83203125" customWidth="1"/>
+    <col min="20" max="20" width="47.5" customWidth="1"/>
+    <col min="22" max="22" width="14.5" customWidth="1"/>
+    <col min="23" max="23" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="62.25" customHeight="1">
+    <row r="1" spans="1:23" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="128"/>
       <c r="B1" s="129" t="s">
         <v>84</v>
@@ -8168,8 +8164,12 @@
       <c r="T1" s="129" t="s">
         <v>840</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="48" customHeight="1">
+      <c r="V1" s="128"/>
+      <c r="W1" s="129" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="97" t="s">
         <v>136</v>
       </c>
@@ -8206,8 +8206,12 @@
         <v>136</v>
       </c>
       <c r="T2" s="105"/>
-    </row>
-    <row r="3" spans="1:20" ht="48" customHeight="1">
+      <c r="V2" s="97" t="s">
+        <v>136</v>
+      </c>
+      <c r="W2" s="105"/>
+    </row>
+    <row r="3" spans="1:23" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="98" t="s">
         <v>165</v>
       </c>
@@ -8248,8 +8252,12 @@
         <v>165</v>
       </c>
       <c r="T3" s="86"/>
-    </row>
-    <row r="4" spans="1:20" ht="55.5" customHeight="1">
+      <c r="V3" s="98" t="s">
+        <v>165</v>
+      </c>
+      <c r="W3" s="86"/>
+    </row>
+    <row r="4" spans="1:23" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="99" t="s">
         <v>198</v>
       </c>
@@ -8286,8 +8294,12 @@
         <v>198</v>
       </c>
       <c r="T4" s="87"/>
-    </row>
-    <row r="5" spans="1:20" ht="57.75" customHeight="1">
+      <c r="V4" s="99" t="s">
+        <v>198</v>
+      </c>
+      <c r="W4" s="87"/>
+    </row>
+    <row r="5" spans="1:23" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="100" t="s">
         <v>233</v>
       </c>
@@ -8324,8 +8336,12 @@
         <v>233</v>
       </c>
       <c r="T5" s="172"/>
-    </row>
-    <row r="6" spans="1:20" ht="78.75" customHeight="1">
+      <c r="V5" s="100" t="s">
+        <v>233</v>
+      </c>
+      <c r="W5" s="172"/>
+    </row>
+    <row r="6" spans="1:23" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="99" t="s">
         <v>256</v>
       </c>
@@ -8357,8 +8373,12 @@
         <v>256</v>
       </c>
       <c r="T6" s="87"/>
-    </row>
-    <row r="7" spans="1:20" ht="106.5" customHeight="1">
+      <c r="V6" s="99" t="s">
+        <v>256</v>
+      </c>
+      <c r="W6" s="87"/>
+    </row>
+    <row r="7" spans="1:23" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="100" t="s">
         <v>289</v>
       </c>
@@ -8397,8 +8417,12 @@
         <v>289</v>
       </c>
       <c r="T7" s="88"/>
-    </row>
-    <row r="8" spans="1:20" ht="49.5" customHeight="1">
+      <c r="V7" s="100" t="s">
+        <v>289</v>
+      </c>
+      <c r="W7" s="88"/>
+    </row>
+    <row r="8" spans="1:23" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="99" t="s">
         <v>328</v>
       </c>
@@ -8439,8 +8463,12 @@
         <v>328</v>
       </c>
       <c r="T8" s="87"/>
-    </row>
-    <row r="9" spans="1:20" ht="77.25" customHeight="1">
+      <c r="V8" s="99" t="s">
+        <v>328</v>
+      </c>
+      <c r="W8" s="87"/>
+    </row>
+    <row r="9" spans="1:23" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="100" t="s">
         <v>370</v>
       </c>
@@ -8481,8 +8509,12 @@
         <v>370</v>
       </c>
       <c r="T9" s="88"/>
-    </row>
-    <row r="10" spans="1:20" ht="96.75" customHeight="1">
+      <c r="V9" s="100" t="s">
+        <v>370</v>
+      </c>
+      <c r="W9" s="88"/>
+    </row>
+    <row r="10" spans="1:23" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="99" t="s">
         <v>413</v>
       </c>
@@ -8523,8 +8555,12 @@
         <v>413</v>
       </c>
       <c r="T10" s="87"/>
-    </row>
-    <row r="11" spans="1:20" ht="36.75" customHeight="1">
+      <c r="V10" s="99" t="s">
+        <v>413</v>
+      </c>
+      <c r="W10" s="87"/>
+    </row>
+    <row r="11" spans="1:23" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="101" t="s">
         <v>456</v>
       </c>
@@ -8565,8 +8601,13 @@
         <v>456</v>
       </c>
       <c r="T11" s="89"/>
-    </row>
-    <row r="13" spans="1:20" ht="234.75" customHeight="1">
+      <c r="V11" s="101" t="s">
+        <v>456</v>
+      </c>
+      <c r="W11" s="89"/>
+    </row>
+    <row r="12" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:23" ht="234.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="130"/>
       <c r="B13" s="131" t="s">
         <v>85</v>
@@ -8592,7 +8633,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="60">
+    <row r="14" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="97" t="s">
         <v>136</v>
       </c>
@@ -8626,11 +8667,9 @@
       <c r="P14" s="97" t="s">
         <v>136</v>
       </c>
-      <c r="Q14" s="96" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="360">
+      <c r="Q14" s="96"/>
+    </row>
+    <row r="15" spans="1:23" ht="335" x14ac:dyDescent="0.2">
       <c r="A15" s="98" t="s">
         <v>165</v>
       </c>
@@ -8664,11 +8703,9 @@
       <c r="P15" s="98" t="s">
         <v>165</v>
       </c>
-      <c r="Q15" s="86" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="90">
+      <c r="Q15" s="86"/>
+    </row>
+    <row r="16" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="99" t="s">
         <v>198</v>
       </c>
@@ -8702,11 +8739,9 @@
       <c r="P16" s="99" t="s">
         <v>198</v>
       </c>
-      <c r="Q16" s="87" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="120">
+      <c r="Q16" s="87"/>
+    </row>
+    <row r="17" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="100" t="s">
         <v>233</v>
       </c>
@@ -8740,11 +8775,9 @@
       <c r="P17" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="Q17" s="88" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="90">
+      <c r="Q17" s="88"/>
+    </row>
+    <row r="18" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A18" s="99" t="s">
         <v>256</v>
       </c>
@@ -8778,7 +8811,7 @@
       </c>
       <c r="Q18" s="87"/>
     </row>
-    <row r="19" spans="1:17" ht="225">
+    <row r="19" spans="1:17" ht="208" x14ac:dyDescent="0.2">
       <c r="A19" s="100" t="s">
         <v>289</v>
       </c>
@@ -8812,11 +8845,9 @@
       <c r="P19" s="100" t="s">
         <v>289</v>
       </c>
-      <c r="Q19" s="166" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="105">
+      <c r="Q19" s="166"/>
+    </row>
+    <row r="20" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A20" s="99" t="s">
         <v>328</v>
       </c>
@@ -8850,11 +8881,9 @@
       <c r="P20" s="99" t="s">
         <v>328</v>
       </c>
-      <c r="Q20" s="87" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="195">
+      <c r="Q20" s="87"/>
+    </row>
+    <row r="21" spans="1:17" ht="160" x14ac:dyDescent="0.2">
       <c r="A21" s="100" t="s">
         <v>370</v>
       </c>
@@ -8888,11 +8917,9 @@
       <c r="P21" s="100" t="s">
         <v>370</v>
       </c>
-      <c r="Q21" s="88" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="120">
+      <c r="Q21" s="88"/>
+    </row>
+    <row r="22" spans="1:17" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="99" t="s">
         <v>413</v>
       </c>
@@ -8926,11 +8953,9 @@
       <c r="P22" s="99" t="s">
         <v>413</v>
       </c>
-      <c r="Q22" s="87" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="79.5" customHeight="1">
+      <c r="Q22" s="87"/>
+    </row>
+    <row r="23" spans="1:17" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="101" t="s">
         <v>456</v>
       </c>
@@ -8964,12 +8989,10 @@
       <c r="P23" s="101" t="s">
         <v>456</v>
       </c>
-      <c r="Q23" s="89" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="15.95" thickBot="1"/>
-    <row r="26" spans="1:17" ht="45">
+      <c r="Q23" s="89"/>
+    </row>
+    <row r="25" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="130"/>
       <c r="B26" s="131" t="s">
         <v>87</v>
@@ -8979,7 +9002,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="97" t="s">
         <v>136</v>
       </c>
@@ -8993,7 +9016,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="30">
+    <row r="28" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="98" t="s">
         <v>165</v>
       </c>
@@ -9007,7 +9030,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="99" t="s">
         <v>198</v>
       </c>
@@ -9021,7 +9044,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="100" t="s">
         <v>233</v>
       </c>
@@ -9035,7 +9058,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="80.099999999999994">
+    <row r="31" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="99" t="s">
         <v>256</v>
       </c>
@@ -9049,7 +9072,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="32.1">
+    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="100" t="s">
         <v>289</v>
       </c>
@@ -9061,7 +9084,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="32.1">
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="99" t="s">
         <v>328</v>
       </c>
@@ -9073,7 +9096,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="60">
+    <row r="34" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="100" t="s">
         <v>370</v>
       </c>
@@ -9087,7 +9110,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30.75">
+    <row r="35" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="99" t="s">
         <v>413</v>
       </c>
@@ -9101,7 +9124,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30.75">
+    <row r="36" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="101" t="s">
         <v>456</v>
       </c>
@@ -9115,56 +9138,56 @@
         <v>415</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.95" thickBot="1"/>
-    <row r="39" spans="1:5" ht="48.95" thickBot="1">
+    <row r="38" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="130"/>
       <c r="B39" s="131" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.95">
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="97" t="s">
         <v>136</v>
       </c>
       <c r="B40" s="95"/>
     </row>
-    <row r="41" spans="1:5" ht="15.95">
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="98" t="s">
         <v>165</v>
       </c>
       <c r="B41" s="86"/>
     </row>
-    <row r="42" spans="1:5" ht="15.95">
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="99" t="s">
         <v>198</v>
       </c>
       <c r="B42" s="87"/>
     </row>
-    <row r="43" spans="1:5" ht="15.95">
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="100" t="s">
         <v>233</v>
       </c>
       <c r="B43" s="88"/>
     </row>
-    <row r="44" spans="1:5" ht="15.95">
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="99" t="s">
         <v>256</v>
       </c>
       <c r="B44" s="87"/>
     </row>
-    <row r="45" spans="1:5" ht="15.95">
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="100" t="s">
         <v>289</v>
       </c>
       <c r="B45" s="88"/>
     </row>
-    <row r="46" spans="1:5" ht="15.95">
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="99" t="s">
         <v>328</v>
       </c>
       <c r="B46" s="87"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="100" t="s">
         <v>370</v>
       </c>
@@ -9172,13 +9195,13 @@
         <v>946</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.95">
+    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="99" t="s">
         <v>413</v>
       </c>
       <c r="B48" s="87"/>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="101" t="s">
         <v>456</v>
       </c>
@@ -9200,43 +9223,43 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.95">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="132"/>
       <c r="B1" s="133" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.95">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="97" t="s">
         <v>136</v>
       </c>
       <c r="B2" s="95"/>
     </row>
-    <row r="3" spans="1:2" ht="15.95">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="98" t="s">
         <v>165</v>
       </c>
       <c r="B3" s="86"/>
     </row>
-    <row r="4" spans="1:2" ht="15.95">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="99" t="s">
         <v>198</v>
       </c>
       <c r="B4" s="87"/>
     </row>
-    <row r="5" spans="1:2" ht="15.95">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="100" t="s">
         <v>233</v>
       </c>
       <c r="B5" s="88"/>
     </row>
-    <row r="6" spans="1:2" ht="15.95">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="99" t="s">
         <v>256</v>
       </c>
@@ -9244,13 +9267,13 @@
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.95">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="100" t="s">
         <v>289</v>
       </c>
       <c r="B7" s="88"/>
     </row>
-    <row r="8" spans="1:2" ht="111.75" customHeight="1">
+    <row r="8" spans="1:2" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="99" t="s">
         <v>328</v>
       </c>
@@ -9258,19 +9281,19 @@
         <v>369</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.95">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="100" t="s">
         <v>370</v>
       </c>
       <c r="B9" s="88"/>
     </row>
-    <row r="10" spans="1:2" ht="15.95">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="99" t="s">
         <v>413</v>
       </c>
       <c r="B10" s="87"/>
     </row>
-    <row r="11" spans="1:2" ht="15.95">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="101" t="s">
         <v>456</v>
       </c>
@@ -9290,12 +9313,12 @@
       <selection pane="bottomLeft" activeCell="BG1" sqref="BG1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="35" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="35" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="35" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" s="25" customFormat="1" ht="176.1">
+    <row r="1" spans="1:62" s="25" customFormat="1" ht="176" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>497</v>
       </c>
@@ -9474,7 +9497,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="320.10000000000002">
+    <row r="2" spans="1:62" ht="320" x14ac:dyDescent="0.2">
       <c r="B2" s="8" t="s">
         <v>136</v>
       </c>
@@ -9576,7 +9599,7 @@
       <c r="BC2" s="36"/>
       <c r="BD2" s="36"/>
     </row>
-    <row r="3" spans="1:62" ht="303.95">
+    <row r="3" spans="1:62" ht="304" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>165</v>
       </c>
@@ -9710,7 +9733,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:62" ht="176.1">
+    <row r="4" spans="1:62" ht="176" x14ac:dyDescent="0.2">
       <c r="B4" s="41" t="s">
         <v>198</v>
       </c>
@@ -9873,7 +9896,7 @@
       <c r="BG4" s="42"/>
       <c r="BH4" s="35"/>
     </row>
-    <row r="5" spans="1:62" ht="96">
+    <row r="5" spans="1:62" ht="96" x14ac:dyDescent="0.2">
       <c r="B5" s="34" t="s">
         <v>233</v>
       </c>
@@ -10032,7 +10055,7 @@
       <c r="BG5" s="43"/>
       <c r="BH5" s="46"/>
     </row>
-    <row r="6" spans="1:62" ht="176.1">
+    <row r="6" spans="1:62" ht="176" x14ac:dyDescent="0.2">
       <c r="B6" s="41" t="s">
         <v>256</v>
       </c>
@@ -10204,7 +10227,7 @@
       <c r="BH6" s="46"/>
       <c r="BI6" s="46"/>
     </row>
-    <row r="7" spans="1:62" ht="409.6">
+    <row r="7" spans="1:62" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B7" s="34" t="s">
         <v>289</v>
       </c>
@@ -10361,7 +10384,7 @@
       <c r="BG7" s="43"/>
       <c r="BH7" s="35"/>
     </row>
-    <row r="8" spans="1:62" ht="192">
+    <row r="8" spans="1:62" ht="192" x14ac:dyDescent="0.2">
       <c r="B8" s="41" t="s">
         <v>328</v>
       </c>
@@ -10526,7 +10549,7 @@
       </c>
       <c r="BH8" s="35"/>
     </row>
-    <row r="9" spans="1:62" ht="128.1">
+    <row r="9" spans="1:62" ht="128" x14ac:dyDescent="0.2">
       <c r="B9" s="34" t="s">
         <v>370</v>
       </c>
@@ -10689,7 +10712,7 @@
       <c r="BG9" s="43"/>
       <c r="BH9" s="35"/>
     </row>
-    <row r="10" spans="1:62" ht="176.1">
+    <row r="10" spans="1:62" ht="176" x14ac:dyDescent="0.2">
       <c r="B10" s="41" t="s">
         <v>413</v>
       </c>
@@ -10852,7 +10875,7 @@
       <c r="BG10" s="42"/>
       <c r="BH10" s="35"/>
     </row>
-    <row r="11" spans="1:62" ht="111.95">
+    <row r="11" spans="1:62" ht="112" x14ac:dyDescent="0.2">
       <c r="B11" s="34" t="s">
         <v>456</v>
       </c>
@@ -11007,7 +11030,7 @@
       <c r="BI11" s="35"/>
       <c r="BJ11" s="35"/>
     </row>
-    <row r="37" spans="1:60" s="7" customFormat="1" ht="80.099999999999994" hidden="1">
+    <row r="37" spans="1:60" s="7" customFormat="1" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" s="7" t="s">
         <v>0</v>
       </c>
@@ -11180,7 +11203,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:60" s="27" customFormat="1" ht="29.25" hidden="1" customHeight="1">
+    <row r="38" spans="1:60" s="27" customFormat="1" ht="29.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
         <v>57</v>
       </c>
@@ -11360,7 +11383,7 @@
       </c>
       <c r="BH38" s="26"/>
     </row>
-    <row r="39" spans="1:60" s="25" customFormat="1" ht="93" hidden="1" customHeight="1">
+    <row r="39" spans="1:60" s="25" customFormat="1" ht="93" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
         <v>63</v>
       </c>
@@ -11539,7 +11562,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:60" s="25" customFormat="1" ht="80.099999999999994" hidden="1">
+    <row r="40" spans="1:60" s="25" customFormat="1" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
         <v>90</v>
       </c>
@@ -11676,7 +11699,7 @@
       <c r="BF40" s="22"/>
       <c r="BG40" s="29"/>
     </row>
-    <row r="41" spans="1:60" s="25" customFormat="1" ht="159.94999999999999" hidden="1">
+    <row r="41" spans="1:60" s="25" customFormat="1" ht="160" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
         <v>109</v>
       </c>
@@ -11789,7 +11812,7 @@
       <c r="BF41" s="22"/>
       <c r="BG41" s="29"/>
     </row>
-    <row r="42" spans="1:60" s="25" customFormat="1" hidden="1">
+    <row r="42" spans="1:60" s="25" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="21"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -11869,20 +11892,20 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" customWidth="1"/>
-    <col min="3" max="3" width="80.42578125" customWidth="1"/>
-    <col min="4" max="4" width="50.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="51.5" customWidth="1"/>
+    <col min="3" max="3" width="80.5" customWidth="1"/>
+    <col min="4" max="4" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.100000000000001">
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="59"/>
       <c r="B2" s="57" t="s">
         <v>110</v>
@@ -11891,7 +11914,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.100000000000001">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="53" t="s">
         <v>136</v>
       </c>
@@ -11902,7 +11925,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="33.950000000000003">
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="53" t="s">
         <v>165</v>
       </c>
@@ -11913,7 +11936,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.100000000000001">
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
         <v>198</v>
       </c>
@@ -11924,7 +11947,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.100000000000001">
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="53" t="s">
         <v>233</v>
       </c>
@@ -11933,7 +11956,7 @@
       </c>
       <c r="C6" s="53"/>
     </row>
-    <row r="7" spans="1:3" ht="17.100000000000001">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="53" t="s">
         <v>256</v>
       </c>
@@ -11944,7 +11967,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="53" t="s">
         <v>289</v>
       </c>
@@ -11955,7 +11978,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.100000000000001">
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
         <v>328</v>
       </c>
@@ -11966,7 +11989,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.100000000000001">
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="53" t="s">
         <v>370</v>
       </c>
@@ -11977,7 +12000,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.100000000000001">
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="53" t="s">
         <v>413</v>
       </c>
@@ -11988,7 +12011,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17.100000000000001">
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>456</v>
       </c>
@@ -11999,13 +12022,13 @@
         <v>458</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.100000000000001">
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="59"/>
       <c r="B15" s="57" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="63.95">
+    <row r="16" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="s">
         <v>136</v>
       </c>
@@ -12013,7 +12036,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="84.95">
+    <row r="17" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A17" s="53" t="s">
         <v>165</v>
       </c>
@@ -12021,7 +12044,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="33.950000000000003">
+    <row r="18" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="53" t="s">
         <v>198</v>
       </c>
@@ -12029,7 +12052,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.100000000000001">
+    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="53" t="s">
         <v>233</v>
       </c>
@@ -12037,7 +12060,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.100000000000001">
+    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="53" t="s">
         <v>256</v>
       </c>
@@ -12045,7 +12068,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17.100000000000001">
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="53" t="s">
         <v>289</v>
       </c>
@@ -12053,7 +12076,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="33.950000000000003">
+    <row r="22" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="53" t="s">
         <v>328</v>
       </c>
@@ -12061,7 +12084,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="68.099999999999994">
+    <row r="23" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="53" t="s">
         <v>370</v>
       </c>
@@ -12069,7 +12092,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1">
+    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="53" t="s">
         <v>413</v>
       </c>
@@ -12077,7 +12100,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="51">
+    <row r="25" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="53" t="s">
         <v>456</v>
       </c>
@@ -12085,13 +12108,13 @@
         <v>526</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17.100000000000001">
+    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="59"/>
       <c r="B28" s="57" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="96">
+    <row r="29" spans="1:2" ht="96" x14ac:dyDescent="0.2">
       <c r="A29" s="53" t="s">
         <v>136</v>
       </c>
@@ -12099,7 +12122,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="17.100000000000001">
+    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="53" t="s">
         <v>165</v>
       </c>
@@ -12107,7 +12130,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="51">
+    <row r="31" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="53" t="s">
         <v>198</v>
       </c>
@@ -12115,7 +12138,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="51">
+    <row r="32" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="53" t="s">
         <v>233</v>
       </c>
@@ -12123,7 +12146,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="51">
+    <row r="33" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="53" t="s">
         <v>256</v>
       </c>
@@ -12131,7 +12154,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="119.1">
+    <row r="34" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A34" s="53" t="s">
         <v>289</v>
       </c>
@@ -12139,7 +12162,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="51">
+    <row r="35" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="53" t="s">
         <v>328</v>
       </c>
@@ -12147,7 +12170,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="51">
+    <row r="36" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A36" s="53" t="s">
         <v>370</v>
       </c>
@@ -12155,7 +12178,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="51">
+    <row r="37" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A37" s="53" t="s">
         <v>413</v>
       </c>
@@ -12163,7 +12186,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="68.099999999999994">
+    <row r="38" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A38" s="53" t="s">
         <v>456</v>
       </c>
@@ -12171,13 +12194,13 @@
         <v>462</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17.100000000000001">
+    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="59"/>
       <c r="B40" s="57" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="80.099999999999994">
+    <row r="41" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A41" s="53" t="s">
         <v>136</v>
       </c>
@@ -12185,7 +12208,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="33.950000000000003">
+    <row r="42" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="53" t="s">
         <v>165</v>
       </c>
@@ -12193,7 +12216,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="17.100000000000001">
+    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="53" t="s">
         <v>198</v>
       </c>
@@ -12201,7 +12224,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17.100000000000001">
+    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="53" t="s">
         <v>233</v>
       </c>
@@ -12209,7 +12232,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17.100000000000001">
+    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="53" t="s">
         <v>256</v>
       </c>
@@ -12217,7 +12240,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="51">
+    <row r="46" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="53" t="s">
         <v>289</v>
       </c>
@@ -12225,7 +12248,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="51">
+    <row r="47" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" s="53" t="s">
         <v>328</v>
       </c>
@@ -12233,7 +12256,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17.100000000000001">
+    <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="53" t="s">
         <v>370</v>
       </c>
@@ -12241,7 +12264,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="33.950000000000003">
+    <row r="49" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="53" t="s">
         <v>413</v>
       </c>
@@ -12249,19 +12272,19 @@
         <v>419</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="17.100000000000001">
+    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="53" t="s">
         <v>456</v>
       </c>
       <c r="B50" s="53"/>
     </row>
-    <row r="53" spans="1:2" ht="31.5" customHeight="1">
+    <row r="53" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="59"/>
       <c r="B53" s="57" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="51">
+    <row r="54" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="53" t="s">
         <v>136</v>
       </c>
@@ -12269,7 +12292,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="120.75" customHeight="1">
+    <row r="55" spans="1:2" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="53" t="s">
         <v>165</v>
       </c>
@@ -12277,7 +12300,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="92.25" customHeight="1">
+    <row r="56" spans="1:2" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="53" t="s">
         <v>198</v>
       </c>
@@ -12285,7 +12308,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="17.100000000000001">
+    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="53" t="s">
         <v>233</v>
       </c>
@@ -12293,7 +12316,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="45" customHeight="1">
+    <row r="58" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="53" t="s">
         <v>256</v>
       </c>
@@ -12301,7 +12324,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="82.5" customHeight="1">
+    <row r="59" spans="1:2" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="53" t="s">
         <v>289</v>
       </c>
@@ -12309,7 +12332,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="68.099999999999994">
+    <row r="60" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A60" s="53" t="s">
         <v>328</v>
       </c>
@@ -12317,7 +12340,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="51">
+    <row r="61" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A61" s="53" t="s">
         <v>370</v>
       </c>
@@ -12325,7 +12348,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="33.950000000000003">
+    <row r="62" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" s="53" t="s">
         <v>413</v>
       </c>
@@ -12333,7 +12356,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="51">
+    <row r="63" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" s="53" t="s">
         <v>456</v>
       </c>
@@ -12341,7 +12364,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="75" customHeight="1">
+    <row r="66" spans="1:3" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="51"/>
       <c r="B66" s="57" t="s">
         <v>129</v>
@@ -12350,7 +12373,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="63.95">
+    <row r="67" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A67" s="57" t="s">
         <v>136</v>
       </c>
@@ -12361,7 +12384,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="17.100000000000001">
+    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="57" t="s">
         <v>165</v>
       </c>
@@ -12372,7 +12395,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="17.100000000000001">
+    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="57" t="s">
         <v>198</v>
       </c>
@@ -12383,7 +12406,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="17.100000000000001">
+    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="57" t="s">
         <v>233</v>
       </c>
@@ -12394,7 +12417,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="51">
+    <row r="71" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="57" t="s">
         <v>256</v>
       </c>
@@ -12405,7 +12428,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="84.95">
+    <row r="72" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A72" s="57" t="s">
         <v>289</v>
       </c>
@@ -12416,7 +12439,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="17.100000000000001">
+    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="57" t="s">
         <v>328</v>
       </c>
@@ -12427,7 +12450,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="33.950000000000003">
+    <row r="74" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="57" t="s">
         <v>370</v>
       </c>
@@ -12438,7 +12461,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="68.099999999999994">
+    <row r="75" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A75" s="57" t="s">
         <v>413</v>
       </c>
@@ -12449,7 +12472,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="17.100000000000001">
+    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="57" t="s">
         <v>456</v>
       </c>
@@ -12473,21 +12496,21 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="52" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
     <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="44.85546875" customWidth="1"/>
+    <col min="5" max="5" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="34.5" customHeight="1">
+    <row r="2" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="59"/>
       <c r="B2" s="57" t="s">
         <v>499</v>
@@ -12502,7 +12525,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" customHeight="1">
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="53" t="s">
         <v>136</v>
       </c>
@@ -12517,7 +12540,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="53" t="s">
         <v>165</v>
       </c>
@@ -12534,7 +12557,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.100000000000001">
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="53" t="s">
         <v>198</v>
       </c>
@@ -12551,7 +12574,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" customHeight="1">
+    <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="53" t="s">
         <v>233</v>
       </c>
@@ -12568,7 +12591,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.100000000000001">
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="53" t="s">
         <v>256</v>
       </c>
@@ -12585,7 +12608,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="33.950000000000003">
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="53" t="s">
         <v>289</v>
       </c>
@@ -12600,7 +12623,7 @@
       </c>
       <c r="E8" s="56"/>
     </row>
-    <row r="9" spans="1:5" ht="17.100000000000001">
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="53" t="s">
         <v>328</v>
       </c>
@@ -12617,7 +12640,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.100000000000001">
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="53" t="s">
         <v>370</v>
       </c>
@@ -12632,7 +12655,7 @@
       </c>
       <c r="E10" s="56"/>
     </row>
-    <row r="11" spans="1:5" ht="19.5" customHeight="1">
+    <row r="11" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="53" t="s">
         <v>413</v>
       </c>
@@ -12647,7 +12670,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="27" customHeight="1">
+    <row r="12" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="53" t="s">
         <v>456</v>
       </c>
@@ -12664,7 +12687,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="51">
+    <row r="15" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="59"/>
       <c r="B15" s="57" t="s">
         <v>102</v>
@@ -12673,7 +12696,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17.100000000000001">
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="53" t="s">
         <v>136</v>
       </c>
@@ -12682,7 +12705,7 @@
       </c>
       <c r="C16" s="53"/>
     </row>
-    <row r="17" spans="1:3" ht="17.100000000000001">
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="53" t="s">
         <v>165</v>
       </c>
@@ -12693,7 +12716,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.100000000000001">
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="53" t="s">
         <v>198</v>
       </c>
@@ -12704,7 +12727,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.100000000000001">
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="53" t="s">
         <v>233</v>
       </c>
@@ -12715,7 +12738,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.100000000000001">
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="53" t="s">
         <v>256</v>
       </c>
@@ -12726,7 +12749,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33.950000000000003">
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="53" t="s">
         <v>289</v>
       </c>
@@ -12737,7 +12760,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="33.950000000000003">
+    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="53" t="s">
         <v>328</v>
       </c>
@@ -12748,7 +12771,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="51">
+    <row r="23" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="53" t="s">
         <v>370</v>
       </c>
@@ -12759,7 +12782,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="68.099999999999994">
+    <row r="24" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="53" t="s">
         <v>413</v>
       </c>
@@ -12770,7 +12793,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="33.950000000000003">
+    <row r="25" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="53" t="s">
         <v>456</v>
       </c>
@@ -12781,19 +12804,19 @@
         <v>482</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="51">
+    <row r="28" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="59"/>
       <c r="B28" s="57" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17.100000000000001">
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="53" t="s">
         <v>136</v>
       </c>
       <c r="B29" s="53"/>
     </row>
-    <row r="30" spans="1:3" ht="17.100000000000001">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="53" t="s">
         <v>165</v>
       </c>
@@ -12801,7 +12824,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17.100000000000001">
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="53" t="s">
         <v>198</v>
       </c>
@@ -12809,7 +12832,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="51">
+    <row r="32" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="53" t="s">
         <v>233</v>
       </c>
@@ -12817,7 +12840,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="17.100000000000001">
+    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="53" t="s">
         <v>256</v>
       </c>
@@ -12825,7 +12848,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17.100000000000001">
+    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="53" t="s">
         <v>289</v>
       </c>
@@ -12833,7 +12856,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17.100000000000001">
+    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="53" t="s">
         <v>328</v>
       </c>
@@ -12841,13 +12864,13 @@
         <v>356</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17.100000000000001">
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="53" t="s">
         <v>370</v>
       </c>
       <c r="B36" s="53"/>
     </row>
-    <row r="37" spans="1:2" ht="17.100000000000001">
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="61" t="s">
         <v>413</v>
       </c>
@@ -12855,7 +12878,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="33.950000000000003">
+    <row r="38" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="53" t="s">
         <v>456</v>
       </c>
@@ -12863,29 +12886,29 @@
         <v>545</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.95">
+    <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="49"/>
       <c r="B39" s="49"/>
     </row>
-    <row r="40" spans="1:2" ht="33.950000000000003">
+    <row r="40" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="59"/>
       <c r="B40" s="57" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17.100000000000001">
+    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="53" t="s">
         <v>136</v>
       </c>
       <c r="B41" s="53"/>
     </row>
-    <row r="42" spans="1:2" ht="17.100000000000001">
+    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="53" t="s">
         <v>165</v>
       </c>
       <c r="B42" s="53"/>
     </row>
-    <row r="43" spans="1:2" ht="17.100000000000001">
+    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="53" t="s">
         <v>198</v>
       </c>
@@ -12893,7 +12916,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17.100000000000001">
+    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="53" t="s">
         <v>233</v>
       </c>
@@ -12901,7 +12924,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="33.950000000000003">
+    <row r="45" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="53" t="s">
         <v>256</v>
       </c>
@@ -12909,13 +12932,13 @@
         <v>278</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17.100000000000001">
+    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="53" t="s">
         <v>289</v>
       </c>
       <c r="B46" s="53"/>
     </row>
-    <row r="47" spans="1:2" ht="33.950000000000003">
+    <row r="47" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="53" t="s">
         <v>328</v>
       </c>
@@ -12923,7 +12946,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="33.950000000000003">
+    <row r="48" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="53" t="s">
         <v>370</v>
       </c>
@@ -12931,7 +12954,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="17.100000000000001">
+    <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="53" t="s">
         <v>413</v>
       </c>
@@ -12939,7 +12962,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="17.100000000000001">
+    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="53" t="s">
         <v>456</v>
       </c>
@@ -12947,7 +12970,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.95">
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="49"/>
     </row>
   </sheetData>
@@ -12963,20 +12986,20 @@
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" style="8" customWidth="1"/>
-    <col min="2" max="2" width="109.42578125" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" customWidth="1"/>
-    <col min="4" max="4" width="64.140625" customWidth="1"/>
+    <col min="2" max="2" width="109.5" customWidth="1"/>
+    <col min="3" max="3" width="56.1640625" customWidth="1"/>
+    <col min="4" max="4" width="64.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.100000000000001">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="50"/>
       <c r="B3" s="57" t="s">
         <v>546</v>
@@ -12988,7 +13011,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.100000000000001">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="52" t="s">
         <v>136</v>
       </c>
@@ -13002,7 +13025,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.100000000000001">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="52" t="s">
         <v>165</v>
       </c>
@@ -13014,7 +13037,7 @@
       </c>
       <c r="D5" s="56"/>
     </row>
-    <row r="6" spans="1:4" ht="17.100000000000001">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="54" t="s">
         <v>198</v>
       </c>
@@ -13026,7 +13049,7 @@
       </c>
       <c r="D6" s="56"/>
     </row>
-    <row r="7" spans="1:4" ht="17.100000000000001">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="55" t="s">
         <v>233</v>
       </c>
@@ -13038,7 +13061,7 @@
       </c>
       <c r="D7" s="56"/>
     </row>
-    <row r="8" spans="1:4" ht="51">
+    <row r="8" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="54" t="s">
         <v>256</v>
       </c>
@@ -13050,7 +13073,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.100000000000001">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
         <v>289</v>
       </c>
@@ -13064,7 +13087,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="33.950000000000003">
+    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="54" t="s">
         <v>328</v>
       </c>
@@ -13076,7 +13099,7 @@
       </c>
       <c r="D10" s="56"/>
     </row>
-    <row r="11" spans="1:4" ht="33.950000000000003">
+    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="55" t="s">
         <v>370</v>
       </c>
@@ -13088,7 +13111,7 @@
       </c>
       <c r="D11" s="56"/>
     </row>
-    <row r="12" spans="1:4" ht="17.100000000000001">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="54" t="s">
         <v>413</v>
       </c>
@@ -13102,7 +13125,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.100000000000001">
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="55" t="s">
         <v>456</v>
       </c>
@@ -13114,13 +13137,13 @@
       </c>
       <c r="D13" s="56"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="50"/>
       <c r="B19" s="51" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="33.950000000000003">
+    <row r="20" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="52" t="s">
         <v>136</v>
       </c>
@@ -13128,7 +13151,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" customHeight="1">
+    <row r="21" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="52" t="s">
         <v>165</v>
       </c>
@@ -13136,7 +13159,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17.100000000000001">
+    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="54" t="s">
         <v>198</v>
       </c>
@@ -13144,7 +13167,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="17.100000000000001">
+    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="55" t="s">
         <v>233</v>
       </c>
@@ -13152,7 +13175,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="33.950000000000003">
+    <row r="24" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="54" t="s">
         <v>256</v>
       </c>
@@ -13160,13 +13183,13 @@
         <v>549</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.95">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="55" t="s">
         <v>289</v>
       </c>
       <c r="B25" s="53"/>
     </row>
-    <row r="26" spans="1:2" ht="33.950000000000003">
+    <row r="26" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="54" t="s">
         <v>328</v>
       </c>
@@ -13174,7 +13197,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="51">
+    <row r="27" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A27" s="55" t="s">
         <v>370</v>
       </c>
@@ -13182,7 +13205,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17.100000000000001">
+    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="54" t="s">
         <v>413</v>
       </c>
@@ -13190,25 +13213,25 @@
         <v>453</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.95">
+    <row r="29" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="55" t="s">
         <v>456</v>
       </c>
       <c r="B29" s="53"/>
     </row>
-    <row r="34" spans="1:2" ht="33.950000000000003">
+    <row r="34" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="50"/>
       <c r="B34" s="57" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.95">
+    <row r="35" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="52" t="s">
         <v>136</v>
       </c>
       <c r="B35" s="53"/>
     </row>
-    <row r="36" spans="1:2" ht="17.100000000000001">
+    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="52" t="s">
         <v>165</v>
       </c>
@@ -13216,7 +13239,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17.100000000000001">
+    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="54" t="s">
         <v>198</v>
       </c>
@@ -13224,7 +13247,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17.100000000000001">
+    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="55" t="s">
         <v>233</v>
       </c>
@@ -13232,7 +13255,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="33.950000000000003">
+    <row r="39" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="54" t="s">
         <v>256</v>
       </c>
@@ -13240,7 +13263,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17.100000000000001">
+    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="55" t="s">
         <v>289</v>
       </c>
@@ -13248,7 +13271,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17.100000000000001">
+    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="54" t="s">
         <v>328</v>
       </c>
@@ -13256,7 +13279,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17.100000000000001">
+    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="55" t="s">
         <v>370</v>
       </c>
@@ -13264,7 +13287,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="33.950000000000003">
+    <row r="43" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="54" t="s">
         <v>413</v>
       </c>
@@ -13272,7 +13295,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17.100000000000001">
+    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="55" t="s">
         <v>456</v>
       </c>
@@ -13293,16 +13316,16 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="57.42578125" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="57.5" customWidth="1"/>
+    <col min="3" max="3" width="75.5" customWidth="1"/>
     <col min="4" max="4" width="56" customWidth="1"/>
-    <col min="5" max="5" width="88.42578125" customWidth="1"/>
+    <col min="5" max="5" width="88.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="67" customFormat="1" ht="32.1">
+    <row r="1" spans="1:5" s="67" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="68"/>
       <c r="B1" s="69" t="s">
         <v>554</v>
@@ -13317,7 +13340,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.95">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
         <v>136</v>
       </c>
@@ -13326,7 +13349,7 @@
       <c r="D2" s="52"/>
       <c r="E2" s="52"/>
     </row>
-    <row r="3" spans="1:5" ht="15.95">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="52" t="s">
         <v>165</v>
       </c>
@@ -13335,7 +13358,7 @@
       <c r="D3" s="52"/>
       <c r="E3" s="52"/>
     </row>
-    <row r="4" spans="1:5" ht="15.95">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="54" t="s">
         <v>198</v>
       </c>
@@ -13344,7 +13367,7 @@
       <c r="D4" s="54"/>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:5" ht="15.95">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
         <v>233</v>
       </c>
@@ -13353,7 +13376,7 @@
       <c r="D5" s="55"/>
       <c r="E5" s="55"/>
     </row>
-    <row r="6" spans="1:5" ht="96" customHeight="1">
+    <row r="6" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="54" t="s">
         <v>256</v>
       </c>
@@ -13368,7 +13391,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.95">
+    <row r="7" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="55" t="s">
         <v>289</v>
       </c>
@@ -13379,7 +13402,7 @@
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
     </row>
-    <row r="8" spans="1:5" ht="19.5" customHeight="1">
+    <row r="8" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="54" t="s">
         <v>328</v>
       </c>
@@ -13390,7 +13413,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.95">
+    <row r="9" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
         <v>370</v>
       </c>
@@ -13401,7 +13424,7 @@
       <c r="D9" s="55"/>
       <c r="E9" s="55"/>
     </row>
-    <row r="10" spans="1:5" ht="15.95">
+    <row r="10" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="54" t="s">
         <v>413</v>
       </c>
@@ -13412,7 +13435,7 @@
       <c r="D10" s="54"/>
       <c r="E10" s="54"/>
     </row>
-    <row r="11" spans="1:5" ht="15.95">
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="55" t="s">
         <v>456</v>
       </c>
@@ -13436,15 +13459,15 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1">
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="83" t="s">
         <v>64</v>
       </c>
@@ -13458,7 +13481,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1">
+    <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="73" t="s">
         <v>136</v>
       </c>
@@ -13472,7 +13495,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30.75" customHeight="1">
+    <row r="3" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="75" t="s">
         <v>165</v>
       </c>
@@ -13486,7 +13509,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="77" t="s">
         <v>198</v>
       </c>
@@ -13500,7 +13523,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.95">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="79" t="s">
         <v>233</v>
       </c>
@@ -13512,7 +13535,7 @@
       </c>
       <c r="D5" s="80"/>
     </row>
-    <row r="6" spans="1:4" ht="15.95">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="77" t="s">
         <v>256</v>
       </c>
@@ -13524,7 +13547,7 @@
       </c>
       <c r="D6" s="78"/>
     </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1">
+    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="79" t="s">
         <v>289</v>
       </c>
@@ -13536,7 +13559,7 @@
       </c>
       <c r="D7" s="80"/>
     </row>
-    <row r="8" spans="1:4" ht="15.95">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="77" t="s">
         <v>328</v>
       </c>
@@ -13548,7 +13571,7 @@
       </c>
       <c r="D8" s="78"/>
     </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1">
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="79" t="s">
         <v>370</v>
       </c>
@@ -13562,7 +13585,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1">
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="77" t="s">
         <v>413</v>
       </c>
@@ -13574,7 +13597,7 @@
       </c>
       <c r="D10" s="78"/>
     </row>
-    <row r="11" spans="1:4" ht="30" customHeight="1">
+    <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="81" t="s">
         <v>456</v>
       </c>
@@ -13599,36 +13622,36 @@
       <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="60.5" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="68.42578125" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="79.7109375" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="60.7109375" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="68.5" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="79.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" customWidth="1"/>
+    <col min="11" max="11" width="60.6640625" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="70.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="80.7109375" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" customWidth="1"/>
-    <col min="20" max="20" width="49.140625" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" customWidth="1"/>
-    <col min="22" max="22" width="22.85546875" customWidth="1"/>
-    <col min="23" max="23" width="74.140625" customWidth="1"/>
-    <col min="25" max="25" width="19.42578125" customWidth="1"/>
-    <col min="26" max="26" width="52.42578125" customWidth="1"/>
+    <col min="14" max="14" width="70.6640625" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="80.6640625" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" customWidth="1"/>
+    <col min="20" max="20" width="49.1640625" customWidth="1"/>
+    <col min="21" max="21" width="6.6640625" customWidth="1"/>
+    <col min="22" max="22" width="22.83203125" customWidth="1"/>
+    <col min="23" max="23" width="74.1640625" customWidth="1"/>
+    <col min="25" max="25" width="19.5" customWidth="1"/>
+    <col min="26" max="26" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30.75">
+    <row r="1" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="107" t="s">
         <v>564</v>
       </c>
@@ -13648,7 +13671,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="135">
+    <row r="2" spans="1:17" ht="128" x14ac:dyDescent="0.2">
       <c r="A2" s="97" t="s">
         <v>136</v>
       </c>
@@ -13668,7 +13691,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="135.75" customHeight="1">
+    <row r="3" spans="1:17" ht="135.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="98" t="s">
         <v>165</v>
       </c>
@@ -13688,7 +13711,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="165">
+    <row r="4" spans="1:17" ht="160" x14ac:dyDescent="0.2">
       <c r="A4" s="99" t="s">
         <v>198</v>
       </c>
@@ -13708,7 +13731,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="90">
+    <row r="5" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="100" t="s">
         <v>233</v>
       </c>
@@ -13728,7 +13751,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="99" t="s">
         <v>256</v>
       </c>
@@ -13742,7 +13765,7 @@
       </c>
       <c r="H6" s="87"/>
     </row>
-    <row r="7" spans="1:17" ht="255">
+    <row r="7" spans="1:17" ht="256" x14ac:dyDescent="0.2">
       <c r="A7" s="100" t="s">
         <v>289</v>
       </c>
@@ -13760,7 +13783,7 @@
       </c>
       <c r="H7" s="88"/>
     </row>
-    <row r="8" spans="1:17" ht="60">
+    <row r="8" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="99" t="s">
         <v>328</v>
       </c>
@@ -13780,7 +13803,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="90">
+    <row r="9" spans="1:17" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="100" t="s">
         <v>370</v>
       </c>
@@ -13800,7 +13823,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="99" t="s">
         <v>413</v>
       </c>
@@ -13814,7 +13837,7 @@
       </c>
       <c r="H10" s="87"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="101" t="s">
         <v>456</v>
       </c>
@@ -13828,7 +13851,7 @@
       </c>
       <c r="H11" s="89"/>
     </row>
-    <row r="14" spans="1:17" ht="71.25" customHeight="1">
+    <row r="14" spans="1:17" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="107" t="s">
         <v>588</v>
       </c>
@@ -13866,7 +13889,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="147.75" customHeight="1">
+    <row r="15" spans="1:17" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="97" t="s">
         <v>136</v>
       </c>
@@ -13909,7 +13932,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="135">
+    <row r="16" spans="1:17" ht="144" x14ac:dyDescent="0.2">
       <c r="A16" s="98" t="s">
         <v>165</v>
       </c>
@@ -13952,7 +13975,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="30">
+    <row r="17" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="99" t="s">
         <v>198</v>
       </c>
@@ -13995,7 +14018,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="45">
+    <row r="18" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="100" t="s">
         <v>233</v>
       </c>
@@ -14036,7 +14059,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="30">
+    <row r="19" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="99" t="s">
         <v>256</v>
       </c>
@@ -14079,7 +14102,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="105">
+    <row r="20" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A20" s="100" t="s">
         <v>289</v>
       </c>
@@ -14122,7 +14145,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="105">
+    <row r="21" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A21" s="99" t="s">
         <v>328</v>
       </c>
@@ -14165,7 +14188,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="45">
+    <row r="22" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="100" t="s">
         <v>370</v>
       </c>
@@ -14208,7 +14231,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="30">
+    <row r="23" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="99" t="s">
         <v>413</v>
       </c>
@@ -14249,7 +14272,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="75">
+    <row r="24" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A24" s="101" t="s">
         <v>456</v>
       </c>
@@ -14290,8 +14313,8 @@
         <v>621</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15.95" thickBot="1"/>
-    <row r="26" spans="1:17" ht="79.5" customHeight="1">
+    <row r="25" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:17" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="110" t="s">
         <v>622</v>
       </c>
@@ -14317,7 +14340,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="94.5" customHeight="1">
+    <row r="27" spans="1:17" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="97" t="s">
         <v>136</v>
       </c>
@@ -14339,7 +14362,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="120">
+    <row r="28" spans="1:17" ht="96" x14ac:dyDescent="0.2">
       <c r="A28" s="98" t="s">
         <v>165</v>
       </c>
@@ -14365,7 +14388,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="105">
+    <row r="29" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A29" s="99" t="s">
         <v>198</v>
       </c>
@@ -14391,7 +14414,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="30">
+    <row r="30" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="100" t="s">
         <v>233</v>
       </c>
@@ -14417,7 +14440,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="45">
+    <row r="31" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="99" t="s">
         <v>256</v>
       </c>
@@ -14443,7 +14466,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="75">
+    <row r="32" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A32" s="100" t="s">
         <v>289</v>
       </c>
@@ -14469,7 +14492,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="45">
+    <row r="33" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="99" t="s">
         <v>328</v>
       </c>
@@ -14495,7 +14518,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="60.75">
+    <row r="34" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="100" t="s">
         <v>370</v>
       </c>
@@ -14521,7 +14544,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="105">
+    <row r="35" spans="1:23" ht="112" x14ac:dyDescent="0.2">
       <c r="A35" s="99" t="s">
         <v>413</v>
       </c>
@@ -14545,7 +14568,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="32.1">
+    <row r="36" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="101" t="s">
         <v>456</v>
       </c>
@@ -14569,7 +14592,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="38" spans="1:23" s="136" customFormat="1" ht="83.25" customHeight="1">
+    <row r="38" spans="1:23" s="136" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="134" t="s">
         <v>646</v>
       </c>
@@ -14620,7 +14643,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="75">
+    <row r="39" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A39" s="97" t="s">
         <v>136</v>
       </c>
@@ -14670,7 +14693,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="75">
+    <row r="40" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A40" s="98" t="s">
         <v>165</v>
       </c>
@@ -14720,7 +14743,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="60">
+    <row r="41" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A41" s="99" t="s">
         <v>198</v>
       </c>
@@ -14770,7 +14793,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="30">
+    <row r="42" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="100" t="s">
         <v>233</v>
       </c>
@@ -14820,7 +14843,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="30">
+    <row r="43" spans="1:23" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="99" t="s">
         <v>256</v>
       </c>
@@ -14868,7 +14891,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="90">
+    <row r="44" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A44" s="100" t="s">
         <v>289</v>
       </c>
@@ -14918,7 +14941,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="90">
+    <row r="45" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A45" s="99" t="s">
         <v>328</v>
       </c>
@@ -14968,7 +14991,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="60">
+    <row r="46" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" s="100" t="s">
         <v>370</v>
       </c>
@@ -15018,7 +15041,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="45">
+    <row r="47" spans="1:23" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="99" t="s">
         <v>413</v>
       </c>
@@ -15066,7 +15089,7 @@
       </c>
       <c r="W47" s="87"/>
     </row>
-    <row r="48" spans="1:23" ht="60">
+    <row r="48" spans="1:23" ht="64" x14ac:dyDescent="0.2">
       <c r="A48" s="101" t="s">
         <v>456</v>
       </c>
@@ -15112,8 +15135,8 @@
       </c>
       <c r="W48" s="89"/>
     </row>
-    <row r="49" spans="1:26" ht="15.95" thickBot="1"/>
-    <row r="50" spans="1:26" s="136" customFormat="1" ht="90">
+    <row r="49" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:26" s="136" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A50" s="134" t="s">
         <v>690</v>
       </c>
@@ -15169,7 +15192,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="60">
+    <row r="51" spans="1:26" ht="64" x14ac:dyDescent="0.2">
       <c r="A51" s="97" t="s">
         <v>136</v>
       </c>
@@ -15225,7 +15248,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="165">
+    <row r="52" spans="1:26" ht="144" x14ac:dyDescent="0.2">
       <c r="A52" s="98" t="s">
         <v>165</v>
       </c>
@@ -15281,7 +15304,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="90">
+    <row r="53" spans="1:26" ht="80" x14ac:dyDescent="0.2">
       <c r="A53" s="99" t="s">
         <v>198</v>
       </c>
@@ -15337,7 +15360,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="54" spans="1:26" ht="45">
+    <row r="54" spans="1:26" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="100" t="s">
         <v>233</v>
       </c>
@@ -15393,7 +15416,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="90">
+    <row r="55" spans="1:26" ht="80" x14ac:dyDescent="0.2">
       <c r="A55" s="99" t="s">
         <v>256</v>
       </c>
@@ -15449,7 +15472,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="165">
+    <row r="56" spans="1:26" ht="144" x14ac:dyDescent="0.2">
       <c r="A56" s="100" t="s">
         <v>289</v>
       </c>
@@ -15505,7 +15528,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="90">
+    <row r="57" spans="1:26" ht="80" x14ac:dyDescent="0.2">
       <c r="A57" s="99" t="s">
         <v>328</v>
       </c>
@@ -15561,7 +15584,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="58" spans="1:26" ht="45">
+    <row r="58" spans="1:26" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="100" t="s">
         <v>370</v>
       </c>
@@ -15617,7 +15640,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="59" spans="1:26" ht="75">
+    <row r="59" spans="1:26" ht="80" x14ac:dyDescent="0.2">
       <c r="A59" s="99" t="s">
         <v>413</v>
       </c>
@@ -15673,7 +15696,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="60" spans="1:26" ht="60">
+    <row r="60" spans="1:26" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="101" t="s">
         <v>456</v>
       </c>
@@ -15725,8 +15748,8 @@
         <v>739</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="15.95" thickBot="1"/>
-    <row r="62" spans="1:26" ht="32.1">
+    <row r="61" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:26" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="113" t="s">
         <v>740</v>
       </c>
@@ -15734,31 +15757,31 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:26" ht="15.95">
+    <row r="63" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="97" t="s">
         <v>136</v>
       </c>
       <c r="B63" s="95"/>
     </row>
-    <row r="64" spans="1:26" ht="15.95">
+    <row r="64" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="98" t="s">
         <v>165</v>
       </c>
       <c r="B64" s="86"/>
     </row>
-    <row r="65" spans="1:2" ht="15.95">
+    <row r="65" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="99" t="s">
         <v>198</v>
       </c>
       <c r="B65" s="87"/>
     </row>
-    <row r="66" spans="1:2" ht="15.95">
+    <row r="66" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="100" t="s">
         <v>233</v>
       </c>
       <c r="B66" s="88"/>
     </row>
-    <row r="67" spans="1:2" ht="15.95">
+    <row r="67" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="99" t="s">
         <v>256</v>
       </c>
@@ -15766,7 +15789,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="100" t="s">
         <v>289</v>
       </c>
@@ -15774,13 +15797,13 @@
         <v>274</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15.95">
+    <row r="69" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="99" t="s">
         <v>328</v>
       </c>
       <c r="B69" s="87"/>
     </row>
-    <row r="70" spans="1:2" ht="15.95">
+    <row r="70" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="100" t="s">
         <v>370</v>
       </c>
@@ -15788,25 +15811,25 @@
         <v>396</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15.95">
+    <row r="71" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="99" t="s">
         <v>413</v>
       </c>
       <c r="B71" s="87"/>
     </row>
-    <row r="72" spans="1:2" ht="15.95">
+    <row r="72" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="101" t="s">
         <v>456</v>
       </c>
       <c r="B72" s="89"/>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75">
         <f>27+8+18</f>
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>741</v>
       </c>
@@ -15829,46 +15852,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF55BB61-3A6F-4270-90C9-AB8A8506205C}">
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H12" workbookViewId="0">
+    <sheetView topLeftCell="H12" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="48.5" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="69.85546875" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
-    <col min="11" max="11" width="49.140625" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="46.7109375" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="45.28515625" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" customWidth="1"/>
-    <col min="19" max="19" width="11.7109375" customWidth="1"/>
-    <col min="20" max="20" width="46.85546875" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" customWidth="1"/>
-    <col min="23" max="23" width="30.7109375" customWidth="1"/>
-    <col min="25" max="25" width="15.140625" customWidth="1"/>
-    <col min="26" max="26" width="28.7109375" customWidth="1"/>
-    <col min="28" max="28" width="14.42578125" customWidth="1"/>
-    <col min="29" max="29" width="37.42578125" customWidth="1"/>
-    <col min="31" max="31" width="13.7109375" customWidth="1"/>
-    <col min="32" max="32" width="68.28515625" customWidth="1"/>
-    <col min="34" max="34" width="20.28515625" customWidth="1"/>
-    <col min="35" max="35" width="50.140625" customWidth="1"/>
+    <col min="5" max="5" width="69.83203125" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" customWidth="1"/>
+    <col min="11" max="11" width="49.1640625" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="46.6640625" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" customWidth="1"/>
+    <col min="17" max="17" width="45.33203125" customWidth="1"/>
+    <col min="18" max="18" width="6.6640625" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" customWidth="1"/>
+    <col min="20" max="20" width="46.83203125" customWidth="1"/>
+    <col min="21" max="21" width="6.6640625" customWidth="1"/>
+    <col min="22" max="22" width="11.6640625" customWidth="1"/>
+    <col min="23" max="23" width="30.6640625" customWidth="1"/>
+    <col min="25" max="25" width="15.1640625" customWidth="1"/>
+    <col min="26" max="26" width="28.6640625" customWidth="1"/>
+    <col min="28" max="28" width="14.5" customWidth="1"/>
+    <col min="29" max="29" width="37.5" customWidth="1"/>
+    <col min="31" max="31" width="13.6640625" customWidth="1"/>
+    <col min="32" max="32" width="68.33203125" customWidth="1"/>
+    <col min="34" max="34" width="20.33203125" customWidth="1"/>
+    <col min="35" max="35" width="50.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="63.95">
+    <row r="1" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="116" t="s">
         <v>742</v>
       </c>
@@ -15894,7 +15917,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="97" t="s">
         <v>136</v>
       </c>
@@ -15920,7 +15943,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="98" t="s">
         <v>165</v>
       </c>
@@ -15946,7 +15969,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.95">
+    <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="99" t="s">
         <v>198</v>
       </c>
@@ -15972,7 +15995,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.95">
+    <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="100" t="s">
         <v>233</v>
       </c>
@@ -15998,7 +16021,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.95">
+    <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="99" t="s">
         <v>256</v>
       </c>
@@ -16024,7 +16047,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="32.1">
+    <row r="7" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="100" t="s">
         <v>289</v>
       </c>
@@ -16050,7 +16073,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="75">
+    <row r="8" spans="1:14" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="99" t="s">
         <v>328</v>
       </c>
@@ -16076,7 +16099,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="100" t="s">
         <v>370</v>
       </c>
@@ -16102,7 +16125,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.95">
+    <row r="10" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="99" t="s">
         <v>413</v>
       </c>
@@ -16128,7 +16151,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="33" thickBot="1">
+    <row r="11" spans="1:14" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="101" t="s">
         <v>456</v>
       </c>
@@ -16154,8 +16177,8 @@
         <v>761</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.95" thickBot="1"/>
-    <row r="13" spans="1:14" ht="63" customHeight="1">
+    <row r="12" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:14" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="118" t="s">
         <v>762</v>
       </c>
@@ -16185,7 +16208,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="97" t="s">
         <v>136</v>
       </c>
@@ -16217,7 +16240,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="22.5" customHeight="1">
+    <row r="15" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="98" t="s">
         <v>165</v>
       </c>
@@ -16249,7 +16272,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="30.75">
+    <row r="16" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="99" t="s">
         <v>198</v>
       </c>
@@ -16281,7 +16304,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="30.75">
+    <row r="17" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="100" t="s">
         <v>233</v>
       </c>
@@ -16313,7 +16336,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.95">
+    <row r="18" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="99" t="s">
         <v>256</v>
       </c>
@@ -16345,7 +16368,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="48">
+    <row r="19" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="100" t="s">
         <v>289</v>
       </c>
@@ -16377,7 +16400,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="32.1">
+    <row r="20" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="99" t="s">
         <v>328</v>
       </c>
@@ -16409,7 +16432,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="45.75">
+    <row r="21" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="100" t="s">
         <v>370</v>
       </c>
@@ -16441,7 +16464,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="159.94999999999999">
+    <row r="22" spans="1:14" ht="160" x14ac:dyDescent="0.2">
       <c r="A22" s="99" t="s">
         <v>413</v>
       </c>
@@ -16473,7 +16496,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="48.95" thickBot="1">
+    <row r="23" spans="1:14" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="101" t="s">
         <v>456</v>
       </c>
@@ -16505,8 +16528,8 @@
         <v>485</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.95" thickBot="1"/>
-    <row r="25" spans="1:14" ht="61.5" customHeight="1" thickBot="1">
+    <row r="24" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:14" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="120"/>
       <c r="B25" s="124" t="s">
         <v>74</v>
@@ -16520,7 +16543,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="45.75">
+    <row r="26" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="97" t="s">
         <v>136</v>
       </c>
@@ -16538,7 +16561,7 @@
       </c>
       <c r="H26" s="159"/>
     </row>
-    <row r="27" spans="1:14" ht="60">
+    <row r="27" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" s="98" t="s">
         <v>165</v>
       </c>
@@ -16558,7 +16581,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="30">
+    <row r="28" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="99" t="s">
         <v>198</v>
       </c>
@@ -16578,7 +16601,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="105">
+    <row r="29" spans="1:14" ht="96" x14ac:dyDescent="0.2">
       <c r="A29" s="100" t="s">
         <v>233</v>
       </c>
@@ -16598,7 +16621,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="111.95">
+    <row r="30" spans="1:14" ht="112" x14ac:dyDescent="0.2">
       <c r="A30" s="99" t="s">
         <v>256</v>
       </c>
@@ -16618,7 +16641,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="75">
+    <row r="31" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" s="100" t="s">
         <v>289</v>
       </c>
@@ -16636,7 +16659,7 @@
       </c>
       <c r="H31" s="162"/>
     </row>
-    <row r="32" spans="1:14" ht="75">
+    <row r="32" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A32" s="99" t="s">
         <v>328</v>
       </c>
@@ -16656,7 +16679,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="30.75">
+    <row r="33" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="100" t="s">
         <v>370</v>
       </c>
@@ -16676,7 +16699,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="90">
+    <row r="34" spans="1:20" ht="96" x14ac:dyDescent="0.2">
       <c r="A34" s="99" t="s">
         <v>413</v>
       </c>
@@ -16694,7 +16717,7 @@
       </c>
       <c r="H34" s="161"/>
     </row>
-    <row r="35" spans="1:20" ht="81" thickBot="1">
+    <row r="35" spans="1:20" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="101" t="s">
         <v>456</v>
       </c>
@@ -16712,8 +16735,8 @@
       </c>
       <c r="H35" s="163"/>
     </row>
-    <row r="36" spans="1:20" ht="15.95" thickBot="1"/>
-    <row r="37" spans="1:20" ht="60">
+    <row r="36" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="155"/>
       <c r="B37" s="156" t="s">
         <v>799</v>
@@ -16743,7 +16766,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="60.75">
+    <row r="38" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="97" t="s">
         <v>136</v>
       </c>
@@ -16787,7 +16810,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="300">
+    <row r="39" spans="1:20" ht="320" x14ac:dyDescent="0.2">
       <c r="A39" s="98" t="s">
         <v>165</v>
       </c>
@@ -16831,7 +16854,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="90">
+    <row r="40" spans="1:20" ht="96" x14ac:dyDescent="0.2">
       <c r="A40" s="99" t="s">
         <v>198</v>
       </c>
@@ -16875,7 +16898,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="60">
+    <row r="41" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A41" s="100" t="s">
         <v>233</v>
       </c>
@@ -16919,7 +16942,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="48">
+    <row r="42" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="99" t="s">
         <v>256</v>
       </c>
@@ -16963,7 +16986,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="144">
+    <row r="43" spans="1:20" ht="144" x14ac:dyDescent="0.2">
       <c r="A43" s="100" t="s">
         <v>289</v>
       </c>
@@ -17003,7 +17026,7 @@
       </c>
       <c r="T43" s="88"/>
     </row>
-    <row r="44" spans="1:20" ht="32.1">
+    <row r="44" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="99" t="s">
         <v>328</v>
       </c>
@@ -17047,7 +17070,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="45.75">
+    <row r="45" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" s="100" t="s">
         <v>370</v>
       </c>
@@ -17091,7 +17114,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="159.94999999999999">
+    <row r="46" spans="1:20" ht="160" x14ac:dyDescent="0.2">
       <c r="A46" s="99" t="s">
         <v>413</v>
       </c>
@@ -17135,7 +17158,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="48.95" thickBot="1">
+    <row r="47" spans="1:20" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="101" t="s">
         <v>456</v>
       </c>
@@ -17179,8 +17202,8 @@
         <v>490</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="15.95" thickBot="1"/>
-    <row r="49" spans="1:5" ht="50.25" customHeight="1" thickBot="1">
+    <row r="48" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:5" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="125"/>
       <c r="B49" s="127" t="s">
         <v>82</v>
@@ -17190,7 +17213,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="97" t="s">
         <v>136</v>
       </c>
@@ -17202,7 +17225,7 @@
       </c>
       <c r="E50" s="121"/>
     </row>
-    <row r="51" spans="1:5" ht="15.95">
+    <row r="51" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="98" t="s">
         <v>165</v>
       </c>
@@ -17214,7 +17237,7 @@
       </c>
       <c r="E51" s="86"/>
     </row>
-    <row r="52" spans="1:5" ht="15.95">
+    <row r="52" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="99" t="s">
         <v>198</v>
       </c>
@@ -17226,7 +17249,7 @@
       </c>
       <c r="E52" s="87"/>
     </row>
-    <row r="53" spans="1:5" ht="15.95">
+    <row r="53" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="100" t="s">
         <v>233</v>
       </c>
@@ -17238,7 +17261,7 @@
       </c>
       <c r="E53" s="88"/>
     </row>
-    <row r="54" spans="1:5" ht="80.099999999999994">
+    <row r="54" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A54" s="99" t="s">
         <v>256</v>
       </c>
@@ -17252,7 +17275,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="48">
+    <row r="55" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="100" t="s">
         <v>289</v>
       </c>
@@ -17264,7 +17287,7 @@
       </c>
       <c r="E55" s="88"/>
     </row>
-    <row r="56" spans="1:5" ht="30">
+    <row r="56" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="99" t="s">
         <v>328</v>
       </c>
@@ -17276,7 +17299,7 @@
       </c>
       <c r="E56" s="87"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="100" t="s">
         <v>370</v>
       </c>
@@ -17290,7 +17313,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.95">
+    <row r="58" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="99" t="s">
         <v>413</v>
       </c>
@@ -17304,7 +17327,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="17.100000000000001" thickBot="1">
+    <row r="59" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="101" t="s">
         <v>456</v>
       </c>
@@ -17326,12 +17349,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17558,19 +17578,46 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1918471B-3575-494A-A238-97D47571C991}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B45268-2425-47D2-956B-0CCF1D385955}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F809E825-8B36-445D-B60D-CFD512FD5558}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F809E825-8B36-445D-B60D-CFD512FD5558}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b3e41e30-95eb-45b9-b657-d2eda7f0eaf6"/>
+    <ds:schemaRef ds:uri="d6ffb985-a7ae-40c0-906d-05d0dcf51054"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B45268-2425-47D2-956B-0CCF1D385955}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1918471B-3575-494A-A238-97D47571C991}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Survey 4th iteration : validation and stakeholders
</commit_message>
<xml_diff>
--- a/Survey.xlsx
+++ b/Survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe/Documents/GitHub/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05C0094-DF20-E44D-9D59-35AC25ED9B96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC3F52E-051D-6F4A-9178-1121518B6FE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1680" windowWidth="32020" windowHeight="16460" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1680" windowWidth="32020" windowHeight="16460" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3342" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3352" uniqueCount="958">
   <si>
     <t>Colonne1</t>
   </si>
@@ -3359,6 +3359,55 @@
   </si>
   <si>
     <t>How does the pilot relate to the stakeholder network?</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>*Professional network of organ advisors, organ builders, organists
+*General public through news sites. E.g. orgelnieuws.nl</t>
+  </si>
+  <si>
+    <t>I listed several organ professionals for the stakeholder network. They seem not to have been invited, though. They might be more interested in the ORGANS pilot than in the project as a whole.</t>
+  </si>
+  <si>
+    <t>*Johan Zoutendijk. Director of Verschueren Orgelbouw
+*Hans Fidom. Full professor organ studies, Free University, Amsterdam
+*Jaap Jan Steensma. Organ advisor
+*Paul Peeters. Organ specialist, University of Gothenburg, Sweden.</t>
+  </si>
+  <si>
+    <t>Via personal academic network.</t>
+  </si>
+  <si>
+    <t>Frans Wiering is on the invitation list for the stake holder network.
+Europeana might be interested
+RISM might be interested
+But I'm not sure whether they have been invited.
+RISM is not on the list, but should be invited.</t>
+  </si>
+  <si>
+    <t>*Academic: dr. Rebekah Ahrendt (Music Historian, Utrecht University)
+*Naomi Barker expressed interest (but she is part of the project).</t>
+  </si>
+  <si>
+    <t>Network of the CNRS, Sorbonne University, Conservatoire National Supérieur de Musique et de Danse de Paris</t>
+  </si>
+  <si>
+    <t>Frans Wiering, Anne-Emmanuelle Ceulemans, Richard Freedman, Dmitri Tymoczko, Kevin Page, Laurent Pugin are on the invitation list for the stake holder network.</t>
+  </si>
+  <si>
+    <t>Frans Wiering
+Anne-Emmanuelle Ceulemans
+Richard Freedman
+Dmitri Tymoczko
+Tim Crawford
+Jesse Rodin
+Anne Cummings
+David Lewis
+Daniele Sabaino
+Katelijne Schiltz
+Laurent Pugin</t>
   </si>
 </sst>
 </file>
@@ -4194,7 +4243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4701,6 +4750,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
@@ -8107,8 +8159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF88C43-E44F-455D-AEE2-5CECD1ADC60A}">
   <dimension ref="A1:W49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N8" zoomScale="111" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" topLeftCell="M13" zoomScale="111" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8128,9 +8180,9 @@
     <col min="13" max="13" width="11.6640625" customWidth="1"/>
     <col min="14" max="14" width="39.5" customWidth="1"/>
     <col min="16" max="16" width="17.5" customWidth="1"/>
-    <col min="17" max="17" width="43.1640625" customWidth="1"/>
+    <col min="17" max="17" width="57.6640625" customWidth="1"/>
     <col min="19" max="19" width="19.83203125" customWidth="1"/>
-    <col min="20" max="20" width="47.5" customWidth="1"/>
+    <col min="20" max="20" width="56.5" customWidth="1"/>
     <col min="22" max="22" width="14.5" customWidth="1"/>
     <col min="23" max="23" width="49.33203125" customWidth="1"/>
   </cols>
@@ -8251,11 +8303,15 @@
       <c r="S3" s="98" t="s">
         <v>165</v>
       </c>
-      <c r="T3" s="86"/>
+      <c r="T3" s="86" t="s">
+        <v>955</v>
+      </c>
       <c r="V3" s="98" t="s">
         <v>165</v>
       </c>
-      <c r="W3" s="86"/>
+      <c r="W3" s="86" t="s">
+        <v>956</v>
+      </c>
     </row>
     <row r="4" spans="1:23" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="99" t="s">
@@ -8554,13 +8610,17 @@
       <c r="S10" s="99" t="s">
         <v>413</v>
       </c>
-      <c r="T10" s="87"/>
+      <c r="T10" s="176" t="s">
+        <v>949</v>
+      </c>
       <c r="V10" s="99" t="s">
         <v>413</v>
       </c>
-      <c r="W10" s="87"/>
-    </row>
-    <row r="11" spans="1:23" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W10" s="87" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="101" t="s">
         <v>456</v>
       </c>
@@ -8600,11 +8660,15 @@
       <c r="S11" s="101" t="s">
         <v>456</v>
       </c>
-      <c r="T11" s="89"/>
+      <c r="T11" s="89" t="s">
+        <v>952</v>
+      </c>
       <c r="V11" s="101" t="s">
         <v>456</v>
       </c>
-      <c r="W11" s="89"/>
+      <c r="W11" s="89" t="s">
+        <v>953</v>
+      </c>
     </row>
     <row r="12" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:23" ht="234.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8703,7 +8767,9 @@
       <c r="P15" s="98" t="s">
         <v>165</v>
       </c>
-      <c r="Q15" s="86"/>
+      <c r="Q15" s="86" t="s">
+        <v>957</v>
+      </c>
     </row>
     <row r="16" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="99" t="s">
@@ -8953,9 +9019,11 @@
       <c r="P22" s="99" t="s">
         <v>413</v>
       </c>
-      <c r="Q22" s="87"/>
-    </row>
-    <row r="23" spans="1:17" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q22" s="87" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="101" t="s">
         <v>456</v>
       </c>
@@ -8989,10 +9057,12 @@
       <c r="P23" s="101" t="s">
         <v>456</v>
       </c>
-      <c r="Q23" s="89"/>
+      <c r="Q23" s="89" t="s">
+        <v>954</v>
+      </c>
     </row>
     <row r="25" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="130"/>
       <c r="B26" s="131" t="s">
         <v>87</v>
@@ -13618,8 +13688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B81DAE-D652-4BB6-8C73-F96210539325}">
   <dimension ref="A1:Z76"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13850,6 +13920,9 @@
         <v>456</v>
       </c>
       <c r="H11" s="89"/>
+      <c r="K11" t="s">
+        <v>948</v>
+      </c>
     </row>
     <row r="14" spans="1:17" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="107" t="s">

</xml_diff>

<commit_message>
question updates according to 6th meeting
</commit_message>
<xml_diff>
--- a/Survey.xlsx
+++ b/Survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe/Documents/GitHub/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210B34CD-5219-2B4D-A7DD-A59427680637}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7EFC45-19AD-B643-BDF6-A6E3D7BB6074}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="820" windowWidth="32020" windowHeight="20180" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="820" windowWidth="32020" windowHeight="20180" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3370" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="982">
   <si>
     <t>Colonne1</t>
   </si>
@@ -3518,6 +3518,12 @@
   </si>
   <si>
     <t xml:space="preserve">*The sources of  MusicBo and MEETUPS are complementary and can mutually enrich the two pilots. </t>
+  </si>
+  <si>
+    <t>To be clarified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where is you demo published? Did you disseminate its availability to target communities? </t>
   </si>
 </sst>
 </file>
@@ -7752,7 +7758,7 @@
       <c r="BG14" s="43"/>
       <c r="BH14" s="35"/>
     </row>
-    <row r="15" spans="1:61" ht="176">
+    <row r="15" spans="1:61" ht="192">
       <c r="B15" s="41" t="s">
         <v>328</v>
       </c>
@@ -8412,10 +8418,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF88C43-E44F-455D-AEE2-5CECD1ADC60A}">
-  <dimension ref="A1:W49"/>
+  <dimension ref="A1:W61"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="110" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8658,7 +8664,9 @@
       <c r="V5" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="W5" s="171"/>
+      <c r="W5" s="87" t="s">
+        <v>980</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="78.75" customHeight="1">
       <c r="A6" s="99" t="s">
@@ -9124,7 +9132,9 @@
       <c r="P17" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="Q17" s="88"/>
+      <c r="Q17" s="88" t="s">
+        <v>980</v>
+      </c>
     </row>
     <row r="18" spans="1:17" ht="80">
       <c r="A18" s="99" t="s">
@@ -9499,74 +9509,141 @@
         <v>415</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="16" thickBot="1"/>
-    <row r="39" spans="1:5" ht="33" thickBot="1">
-      <c r="A39" s="129"/>
-      <c r="B39" s="130" t="s">
+    <row r="37" spans="1:5" ht="16" thickBot="1"/>
+    <row r="38" spans="1:5" ht="33" thickBot="1">
+      <c r="A38" s="129"/>
+      <c r="B38" s="130" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16">
+      <c r="A39" s="97" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" s="95"/>
+    </row>
+    <row r="40" spans="1:5" ht="16">
+      <c r="A40" s="98" t="s">
+        <v>165</v>
+      </c>
+      <c r="B40" s="86"/>
+    </row>
+    <row r="41" spans="1:5" ht="16">
+      <c r="A41" s="99" t="s">
+        <v>198</v>
+      </c>
+      <c r="B41" s="87"/>
+    </row>
+    <row r="42" spans="1:5" ht="16">
+      <c r="A42" s="100" t="s">
+        <v>233</v>
+      </c>
+      <c r="B42" s="88"/>
+    </row>
+    <row r="43" spans="1:5" ht="16">
+      <c r="A43" s="99" t="s">
+        <v>256</v>
+      </c>
+      <c r="B43" s="87"/>
+    </row>
+    <row r="44" spans="1:5" ht="16">
+      <c r="A44" s="100" t="s">
+        <v>289</v>
+      </c>
+      <c r="B44" s="88"/>
+    </row>
+    <row r="45" spans="1:5" ht="16">
+      <c r="A45" s="99" t="s">
+        <v>328</v>
+      </c>
+      <c r="B45" s="87"/>
+    </row>
+    <row r="46" spans="1:5" ht="16">
+      <c r="A46" s="100" t="s">
+        <v>370</v>
+      </c>
+      <c r="B46" s="88"/>
+    </row>
+    <row r="47" spans="1:5" ht="16">
+      <c r="A47" s="99" t="s">
+        <v>413</v>
+      </c>
+      <c r="B47" s="87"/>
+    </row>
+    <row r="48" spans="1:5" ht="17" thickBot="1">
+      <c r="A48" s="101" t="s">
+        <v>456</v>
+      </c>
+      <c r="B48" s="89"/>
+    </row>
+    <row r="50" spans="1:2" ht="16" thickBot="1"/>
+    <row r="51" spans="1:2" ht="33" thickBot="1">
+      <c r="A51" s="129"/>
+      <c r="B51" s="130" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16">
-      <c r="A40" s="97" t="s">
+    <row r="52" spans="1:2" ht="16">
+      <c r="A52" s="97" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="95"/>
-    </row>
-    <row r="41" spans="1:5" ht="16">
-      <c r="A41" s="98" t="s">
+      <c r="B52" s="95"/>
+    </row>
+    <row r="53" spans="1:2" ht="16">
+      <c r="A53" s="98" t="s">
         <v>165</v>
       </c>
-      <c r="B41" s="86"/>
-    </row>
-    <row r="42" spans="1:5" ht="16">
-      <c r="A42" s="99" t="s">
+      <c r="B53" s="86"/>
+    </row>
+    <row r="54" spans="1:2" ht="16">
+      <c r="A54" s="99" t="s">
         <v>198</v>
       </c>
-      <c r="B42" s="87"/>
-    </row>
-    <row r="43" spans="1:5" ht="16">
-      <c r="A43" s="100" t="s">
+      <c r="B54" s="87"/>
+    </row>
+    <row r="55" spans="1:2" ht="16">
+      <c r="A55" s="100" t="s">
         <v>233</v>
       </c>
-      <c r="B43" s="88"/>
-    </row>
-    <row r="44" spans="1:5" ht="16">
-      <c r="A44" s="99" t="s">
+      <c r="B55" s="88"/>
+    </row>
+    <row r="56" spans="1:2" ht="16">
+      <c r="A56" s="99" t="s">
         <v>256</v>
       </c>
-      <c r="B44" s="87"/>
-    </row>
-    <row r="45" spans="1:5" ht="16">
-      <c r="A45" s="100" t="s">
+      <c r="B56" s="87"/>
+    </row>
+    <row r="57" spans="1:2" ht="16">
+      <c r="A57" s="100" t="s">
         <v>289</v>
       </c>
-      <c r="B45" s="88"/>
-    </row>
-    <row r="46" spans="1:5" ht="16">
-      <c r="A46" s="99" t="s">
+      <c r="B57" s="88"/>
+    </row>
+    <row r="58" spans="1:2" ht="16">
+      <c r="A58" s="99" t="s">
         <v>328</v>
       </c>
-      <c r="B46" s="87"/>
-    </row>
-    <row r="47" spans="1:5" ht="16">
-      <c r="A47" s="100" t="s">
+      <c r="B58" s="87"/>
+    </row>
+    <row r="59" spans="1:2" ht="16">
+      <c r="A59" s="100" t="s">
         <v>370</v>
       </c>
-      <c r="B47" s="88" t="s">
+      <c r="B59" s="88" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="16">
-      <c r="A48" s="99" t="s">
+    <row r="60" spans="1:2" ht="16">
+      <c r="A60" s="99" t="s">
         <v>413</v>
       </c>
-      <c r="B48" s="87"/>
-    </row>
-    <row r="49" spans="1:2" ht="16">
-      <c r="A49" s="101" t="s">
+      <c r="B60" s="87"/>
+    </row>
+    <row r="61" spans="1:2" ht="16">
+      <c r="A61" s="101" t="s">
         <v>456</v>
       </c>
-      <c r="B49" s="89"/>
+      <c r="B61" s="89"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9581,7 +9658,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10745,7 +10822,7 @@
       <c r="BG7" s="43"/>
       <c r="BH7" s="35"/>
     </row>
-    <row r="8" spans="1:62" ht="176">
+    <row r="8" spans="1:62" ht="192">
       <c r="B8" s="41" t="s">
         <v>328</v>
       </c>
@@ -13979,7 +14056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B81DAE-D652-4BB6-8C73-F96210539325}">
   <dimension ref="A1:Z76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -16216,8 +16293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF55BB61-3A6F-4270-90C9-AB8A8506205C}">
   <dimension ref="B1:U59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="87" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView showGridLines="0" zoomScale="87" workbookViewId="0">
+      <selection activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -17522,7 +17599,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="47" spans="2:21" ht="65" thickBot="1">
+    <row r="47" spans="2:21" ht="49" thickBot="1">
       <c r="B47" s="101" t="s">
         <v>456</v>
       </c>
@@ -17625,7 +17702,7 @@
       </c>
       <c r="F53" s="88"/>
     </row>
-    <row r="54" spans="2:6" ht="128">
+    <row r="54" spans="2:6" ht="112">
       <c r="B54" s="99" t="s">
         <v>256</v>
       </c>
@@ -17713,12 +17790,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17945,15 +18019,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1918471B-3575-494A-A238-97D47571C991}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B45268-2425-47D2-956B-0CCF1D385955}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17978,10 +18056,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98B45268-2425-47D2-956B-0CCF1D385955}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1918471B-3575-494A-A238-97D47571C991}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>